<commit_message>
Excel Object and Logger Object
</commit_message>
<xml_diff>
--- a/com.romaremedysolutions/RemedyMetadata/RemedySignUpMetadata.xlsx
+++ b/com.romaremedysolutions/RemedyMetadata/RemedySignUpMetadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="23820" windowHeight="10110" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="23820" windowHeight="10110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -2287,6 +2287,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2371,6 +2372,126 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2383,127 +2504,6 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2829,41 +2829,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="102" t="s">
         <v>284</v>
       </c>
-      <c r="E1" s="102"/>
-      <c r="F1" s="113" t="s">
+      <c r="E1" s="103"/>
+      <c r="F1" s="114" t="s">
         <v>285</v>
       </c>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="107" t="s">
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="108"/>
+      <c r="L1" s="109"/>
     </row>
     <row r="2" spans="4:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="105"/>
       <c r="F2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="115" t="s">
+      <c r="G2" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="110"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="111"/>
       <c r="S2" s="26"/>
     </row>
     <row r="3" spans="4:19" ht="16.5" thickBot="1">
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="46" t="s">
         <v>5</v>
       </c>
@@ -2875,15 +2875,15 @@
       <c r="J3" s="50">
         <v>5.2</v>
       </c>
-      <c r="K3" s="109"/>
-      <c r="L3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="111"/>
       <c r="Q3" s="40"/>
       <c r="R3" s="41"/>
       <c r="S3" s="42"/>
     </row>
     <row r="4" spans="4:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D4" s="103"/>
-      <c r="E4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="105"/>
       <c r="F4" s="46" t="s">
         <v>3</v>
       </c>
@@ -2893,13 +2893,13 @@
       <c r="H4" s="50"/>
       <c r="I4" s="48"/>
       <c r="J4" s="48"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="110"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="111"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="4:19" ht="16.5" thickBot="1">
-      <c r="D5" s="105"/>
-      <c r="E5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="47" t="s">
         <v>4</v>
       </c>
@@ -2909,8 +2909,8 @@
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="113"/>
       <c r="Q5" s="40"/>
       <c r="R5" s="41"/>
       <c r="S5" s="42"/>
@@ -2959,10 +2959,10 @@
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="96" t="s">
         <v>286</v>
       </c>
-      <c r="E11" s="96"/>
+      <c r="E11" s="97"/>
       <c r="F11" s="85" t="s">
         <v>288</v>
       </c>
@@ -2978,8 +2978,8 @@
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D12" s="91"/>
-      <c r="E12" s="97"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="98"/>
       <c r="F12" s="86" t="s">
         <v>291</v>
       </c>
@@ -2995,8 +2995,8 @@
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D13" s="91"/>
-      <c r="E13" s="97"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="98"/>
       <c r="F13" s="86" t="s">
         <v>292</v>
       </c>
@@ -3012,8 +3012,8 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D14" s="98"/>
-      <c r="E14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="100"/>
       <c r="F14" s="86" t="s">
         <v>294</v>
       </c>
@@ -3029,10 +3029,10 @@
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="90" t="s">
         <v>300</v>
       </c>
-      <c r="E15" s="90"/>
+      <c r="E15" s="91"/>
       <c r="F15" s="87"/>
       <c r="G15" s="15"/>
       <c r="H15" s="1"/>
@@ -3044,8 +3044,8 @@
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D16" s="91"/>
-      <c r="E16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="93"/>
       <c r="F16" s="86" t="s">
         <v>287</v>
       </c>
@@ -3061,8 +3061,8 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D17" s="91"/>
-      <c r="E17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="93"/>
       <c r="F17" s="86" t="s">
         <v>299</v>
       </c>
@@ -3078,8 +3078,8 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D18" s="98"/>
-      <c r="E18" s="100"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="101"/>
       <c r="F18" s="86"/>
       <c r="G18" s="83"/>
       <c r="H18" s="1"/>
@@ -3091,10 +3091,10 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="90" t="s">
         <v>296</v>
       </c>
-      <c r="E19" s="90"/>
+      <c r="E19" s="91"/>
       <c r="F19" s="87" t="s">
         <v>278</v>
       </c>
@@ -3110,8 +3110,8 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D20" s="91"/>
-      <c r="E20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="93"/>
       <c r="F20" s="87" t="s">
         <v>279</v>
       </c>
@@ -3127,8 +3127,8 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="4:19" ht="15.75" customHeight="1">
-      <c r="D21" s="91"/>
-      <c r="E21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="93"/>
       <c r="F21" s="87" t="s">
         <v>281</v>
       </c>
@@ -3144,8 +3144,8 @@
       <c r="O21" s="1"/>
     </row>
     <row r="22" spans="4:19" ht="16.5" thickBot="1">
-      <c r="D22" s="93"/>
-      <c r="E22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="95"/>
       <c r="F22" s="88" t="s">
         <v>297</v>
       </c>
@@ -4569,8 +4569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4578,7 +4578,7 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4596,10 +4596,10 @@
         <v>302</v>
       </c>
       <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
         <v>303</v>
-      </c>
-      <c r="F1" t="s">
-        <v>203</v>
       </c>
       <c r="G1" t="s">
         <v>205</v>
@@ -4612,7 +4612,7 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>204</v>
       </c>
     </row>
@@ -4623,7 +4623,7 @@
       <c r="C3" t="s">
         <v>206</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4634,7 +4634,7 @@
       <c r="C4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4645,7 +4645,7 @@
       <c r="C5" t="s">
         <v>209</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4656,7 +4656,7 @@
       <c r="C6" t="s">
         <v>210</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4667,7 +4667,7 @@
       <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4678,7 +4678,7 @@
       <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4689,7 +4689,7 @@
       <c r="C9" t="s">
         <v>89</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4700,7 +4700,7 @@
       <c r="C10" t="s">
         <v>95</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       <c r="C11" t="s">
         <v>262</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4722,7 +4722,7 @@
       <c r="C12" t="s">
         <v>263</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4733,7 +4733,7 @@
       <c r="C13" t="s">
         <v>264</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4744,7 +4744,7 @@
       <c r="C14" t="s">
         <v>265</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4755,7 +4755,7 @@
       <c r="C15" t="s">
         <v>266</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4766,183 +4766,183 @@
       <c r="C16" t="s">
         <v>267</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:5">
       <c r="B17" t="s">
         <v>246</v>
       </c>
       <c r="C17" t="s">
         <v>216</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E17" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:5">
       <c r="B18" t="s">
         <v>247</v>
       </c>
       <c r="C18" t="s">
         <v>217</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:5">
       <c r="B19" t="s">
         <v>248</v>
       </c>
       <c r="C19" t="s">
         <v>268</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E19" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:5">
       <c r="B20" t="s">
         <v>249</v>
       </c>
       <c r="C20" t="s">
         <v>268</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:5">
       <c r="B21" t="s">
         <v>250</v>
       </c>
       <c r="C21" t="s">
         <v>268</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E21" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
         <v>251</v>
       </c>
       <c r="C22" t="s">
         <v>268</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E22" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:5">
       <c r="B23" t="s">
         <v>252</v>
       </c>
       <c r="C23" t="s">
         <v>268</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E23" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
         <v>253</v>
       </c>
       <c r="C24" t="s">
         <v>268</v>
       </c>
-      <c r="F24" t="s">
+      <c r="E24" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>254</v>
       </c>
       <c r="C25" t="s">
         <v>222</v>
       </c>
-      <c r="F25" t="s">
+      <c r="E25" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:5">
       <c r="B26" t="s">
         <v>255</v>
       </c>
       <c r="C26" t="s">
         <v>268</v>
       </c>
-      <c r="F26" t="s">
+      <c r="E26" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:5">
       <c r="B27" t="s">
         <v>256</v>
       </c>
       <c r="C27" t="s">
         <v>223</v>
       </c>
-      <c r="F27" t="s">
+      <c r="E27" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:5">
       <c r="B28" t="s">
         <v>257</v>
       </c>
       <c r="C28" t="s">
         <v>227</v>
       </c>
-      <c r="F28" t="s">
+      <c r="E28" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:5">
       <c r="B29" t="s">
         <v>258</v>
       </c>
       <c r="C29" t="s">
         <v>268</v>
       </c>
-      <c r="F29" t="s">
+      <c r="E29" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:5">
       <c r="B30" t="s">
         <v>259</v>
       </c>
       <c r="C30" t="s">
         <v>268</v>
       </c>
-      <c r="F30" t="s">
+      <c r="E30" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:5">
       <c r="B31" t="s">
         <v>260</v>
       </c>
       <c r="C31" t="s">
         <v>268</v>
       </c>
-      <c r="F31" t="s">
+      <c r="E31" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:5">
       <c r="B32" t="s">
         <v>261</v>
       </c>
       <c r="C32" t="s">
         <v>276</v>
       </c>
-      <c r="F32" t="s">
+      <c r="E32" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5398,7 +5398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A7:R280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -5413,18 +5413,18 @@
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" ht="19.5" thickBot="1">
-      <c r="C8" s="118" t="s">
+      <c r="C8" s="159" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="120"/>
+      <c r="D8" s="160"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="160"/>
+      <c r="K8" s="160"/>
+      <c r="L8" s="161"/>
       <c r="O8" s="18"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -5447,21 +5447,21 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B10" s="117" t="s">
+      <c r="B10" s="158" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="117"/>
-      <c r="G10" s="117"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="117"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
+      <c r="C10" s="158"/>
+      <c r="D10" s="158"/>
+      <c r="E10" s="158"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="158"/>
+      <c r="H10" s="158"/>
+      <c r="I10" s="158"/>
+      <c r="J10" s="158"/>
+      <c r="K10" s="158"/>
+      <c r="L10" s="158"/>
+      <c r="M10" s="158"/>
+      <c r="N10" s="158"/>
       <c r="O10" s="18"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -5472,15 +5472,15 @@
       <c r="B11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="121" t="s">
+      <c r="C11" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="123"/>
+      <c r="D11" s="142"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="142"/>
+      <c r="G11" s="142"/>
+      <c r="H11" s="142"/>
+      <c r="I11" s="143"/>
       <c r="J11" s="11" t="s">
         <v>10</v>
       </c>
@@ -5499,25 +5499,25 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="68"/>
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="135"/>
-      <c r="G12" s="124" t="s">
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="125"/>
-      <c r="I12" s="136"/>
-      <c r="J12" s="124" t="s">
+      <c r="H12" s="135"/>
+      <c r="I12" s="137"/>
+      <c r="J12" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="125"/>
-      <c r="L12" s="125"/>
-      <c r="M12" s="125"/>
-      <c r="N12" s="126"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="135"/>
+      <c r="M12" s="135"/>
+      <c r="N12" s="136"/>
       <c r="O12" s="20"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -5588,15 +5588,15 @@
       <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="121" t="s">
+      <c r="C16" s="141" t="s">
         <v>206</v>
       </c>
-      <c r="D16" s="122"/>
-      <c r="E16" s="122"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="122"/>
-      <c r="H16" s="122"/>
-      <c r="I16" s="123"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="142"/>
+      <c r="H16" s="142"/>
+      <c r="I16" s="143"/>
       <c r="J16" s="11" t="s">
         <v>10</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>12</v>
       </c>
       <c r="O16" s="19"/>
-      <c r="P16" s="161" t="s">
+      <c r="P16" s="89" t="s">
         <v>304</v>
       </c>
       <c r="Q16" s="1"/>
@@ -5617,27 +5617,27 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="68"/>
-      <c r="B17" s="133" t="s">
+      <c r="B17" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-      <c r="F17" s="135"/>
-      <c r="G17" s="124" t="s">
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="125"/>
-      <c r="I17" s="136"/>
-      <c r="J17" s="124" t="s">
+      <c r="H17" s="135"/>
+      <c r="I17" s="137"/>
+      <c r="J17" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="125"/>
-      <c r="L17" s="125"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="126"/>
+      <c r="K17" s="135"/>
+      <c r="L17" s="135"/>
+      <c r="M17" s="135"/>
+      <c r="N17" s="136"/>
       <c r="O17" s="20"/>
-      <c r="P17" s="161"/>
+      <c r="P17" s="89"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
@@ -5665,7 +5665,7 @@
       <c r="M18" s="128"/>
       <c r="N18" s="129"/>
       <c r="O18" s="21"/>
-      <c r="P18" s="161"/>
+      <c r="P18" s="89"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
@@ -5691,13 +5691,13 @@
       <c r="M19" s="131"/>
       <c r="N19" s="132"/>
       <c r="O19" s="21"/>
-      <c r="P19" s="161"/>
+      <c r="P19" s="89"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" thickBot="1">
       <c r="O20" s="18"/>
-      <c r="P20" s="161"/>
+      <c r="P20" s="89"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
@@ -5706,15 +5706,15 @@
       <c r="B21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="141" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="122"/>
-      <c r="E21" s="122"/>
-      <c r="F21" s="122"/>
-      <c r="G21" s="122"/>
-      <c r="H21" s="122"/>
-      <c r="I21" s="123"/>
+      <c r="D21" s="142"/>
+      <c r="E21" s="142"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="142"/>
+      <c r="I21" s="143"/>
       <c r="J21" s="11" t="s">
         <v>10</v>
       </c>
@@ -5727,33 +5727,33 @@
         <v>12</v>
       </c>
       <c r="O21" s="19"/>
-      <c r="P21" s="161"/>
+      <c r="P21" s="89"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="68"/>
-      <c r="B22" s="133" t="s">
+      <c r="B22" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="134"/>
-      <c r="D22" s="134"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="135"/>
-      <c r="G22" s="124" t="s">
+      <c r="C22" s="139"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="125"/>
-      <c r="I22" s="136"/>
-      <c r="J22" s="124" t="s">
+      <c r="H22" s="135"/>
+      <c r="I22" s="137"/>
+      <c r="J22" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="125"/>
-      <c r="L22" s="125"/>
-      <c r="M22" s="125"/>
-      <c r="N22" s="126"/>
+      <c r="K22" s="135"/>
+      <c r="L22" s="135"/>
+      <c r="M22" s="135"/>
+      <c r="N22" s="136"/>
       <c r="O22" s="20"/>
-      <c r="P22" s="161"/>
+      <c r="P22" s="89"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
@@ -5781,7 +5781,7 @@
       <c r="M23" s="128"/>
       <c r="N23" s="129"/>
       <c r="O23" s="21"/>
-      <c r="P23" s="161"/>
+      <c r="P23" s="89"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
@@ -5807,13 +5807,13 @@
       <c r="M24" s="131"/>
       <c r="N24" s="132"/>
       <c r="O24" s="21"/>
-      <c r="P24" s="161"/>
+      <c r="P24" s="89"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1">
       <c r="O25" s="18"/>
-      <c r="P25" s="161"/>
+      <c r="P25" s="89"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
@@ -5822,15 +5822,15 @@
       <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="121" t="s">
+      <c r="C26" s="141" t="s">
         <v>209</v>
       </c>
-      <c r="D26" s="122"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="123"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="142"/>
+      <c r="I26" s="143"/>
       <c r="J26" s="11" t="s">
         <v>10</v>
       </c>
@@ -5843,33 +5843,33 @@
         <v>12</v>
       </c>
       <c r="O26" s="18"/>
-      <c r="P26" s="161"/>
+      <c r="P26" s="89"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="68"/>
-      <c r="B27" s="133" t="s">
+      <c r="B27" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="134"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="135"/>
-      <c r="G27" s="124" t="s">
+      <c r="C27" s="139"/>
+      <c r="D27" s="139"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="125"/>
-      <c r="I27" s="136"/>
-      <c r="J27" s="124" t="s">
+      <c r="H27" s="135"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="125"/>
-      <c r="L27" s="125"/>
-      <c r="M27" s="125"/>
-      <c r="N27" s="126"/>
+      <c r="K27" s="135"/>
+      <c r="L27" s="135"/>
+      <c r="M27" s="135"/>
+      <c r="N27" s="136"/>
       <c r="O27" s="19"/>
-      <c r="P27" s="161"/>
+      <c r="P27" s="89"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
@@ -5897,7 +5897,7 @@
       <c r="M28" s="128"/>
       <c r="N28" s="129"/>
       <c r="O28" s="20"/>
-      <c r="P28" s="161"/>
+      <c r="P28" s="89"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
@@ -5923,13 +5923,13 @@
       <c r="M29" s="131"/>
       <c r="N29" s="132"/>
       <c r="O29" s="21"/>
-      <c r="P29" s="161"/>
+      <c r="P29" s="89"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" thickBot="1">
       <c r="O30" s="21"/>
-      <c r="P30" s="161"/>
+      <c r="P30" s="89"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
@@ -5938,15 +5938,15 @@
       <c r="B31" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="121" t="s">
+      <c r="C31" s="141" t="s">
         <v>210</v>
       </c>
-      <c r="D31" s="122"/>
-      <c r="E31" s="122"/>
-      <c r="F31" s="122"/>
-      <c r="G31" s="122"/>
-      <c r="H31" s="122"/>
-      <c r="I31" s="123"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="143"/>
       <c r="J31" s="11" t="s">
         <v>10</v>
       </c>
@@ -5959,33 +5959,33 @@
         <v>12</v>
       </c>
       <c r="O31" s="18"/>
-      <c r="P31" s="161"/>
+      <c r="P31" s="89"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="68"/>
-      <c r="B32" s="133" t="s">
+      <c r="B32" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="135"/>
-      <c r="G32" s="124" t="s">
+      <c r="C32" s="139"/>
+      <c r="D32" s="139"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="125"/>
-      <c r="I32" s="136"/>
-      <c r="J32" s="124" t="s">
+      <c r="H32" s="135"/>
+      <c r="I32" s="137"/>
+      <c r="J32" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K32" s="125"/>
-      <c r="L32" s="125"/>
-      <c r="M32" s="125"/>
-      <c r="N32" s="126"/>
+      <c r="K32" s="135"/>
+      <c r="L32" s="135"/>
+      <c r="M32" s="135"/>
+      <c r="N32" s="136"/>
       <c r="O32" s="19"/>
-      <c r="P32" s="161"/>
+      <c r="P32" s="89"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
@@ -6056,15 +6056,15 @@
       <c r="B36" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="121" t="s">
+      <c r="C36" s="141" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="122"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="122"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="122"/>
-      <c r="I36" s="123"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="143"/>
       <c r="J36" s="11" t="s">
         <v>10</v>
       </c>
@@ -6085,25 +6085,25 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="68"/>
-      <c r="B37" s="133" t="s">
+      <c r="B37" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="134"/>
-      <c r="D37" s="134"/>
-      <c r="E37" s="134"/>
-      <c r="F37" s="135"/>
-      <c r="G37" s="124" t="s">
+      <c r="C37" s="139"/>
+      <c r="D37" s="139"/>
+      <c r="E37" s="139"/>
+      <c r="F37" s="140"/>
+      <c r="G37" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="125"/>
-      <c r="I37" s="136"/>
-      <c r="J37" s="124" t="s">
+      <c r="H37" s="135"/>
+      <c r="I37" s="137"/>
+      <c r="J37" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K37" s="125"/>
-      <c r="L37" s="125"/>
-      <c r="M37" s="125"/>
-      <c r="N37" s="126"/>
+      <c r="K37" s="135"/>
+      <c r="L37" s="135"/>
+      <c r="M37" s="135"/>
+      <c r="N37" s="136"/>
       <c r="O37" s="19"/>
       <c r="P37" s="1" t="s">
         <v>199</v>
@@ -6176,15 +6176,15 @@
       <c r="B41" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="121" t="s">
+      <c r="C41" s="141" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="122"/>
-      <c r="E41" s="122"/>
-      <c r="F41" s="122"/>
-      <c r="G41" s="122"/>
-      <c r="H41" s="122"/>
-      <c r="I41" s="123"/>
+      <c r="D41" s="142"/>
+      <c r="E41" s="142"/>
+      <c r="F41" s="142"/>
+      <c r="G41" s="142"/>
+      <c r="H41" s="142"/>
+      <c r="I41" s="143"/>
       <c r="J41" s="11" t="s">
         <v>10</v>
       </c>
@@ -6203,25 +6203,25 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="68"/>
-      <c r="B42" s="133" t="s">
+      <c r="B42" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="134"/>
-      <c r="D42" s="134"/>
-      <c r="E42" s="134"/>
-      <c r="F42" s="135"/>
-      <c r="G42" s="124" t="s">
+      <c r="C42" s="139"/>
+      <c r="D42" s="139"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="140"/>
+      <c r="G42" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="125"/>
-      <c r="I42" s="136"/>
-      <c r="J42" s="124" t="s">
+      <c r="H42" s="135"/>
+      <c r="I42" s="137"/>
+      <c r="J42" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K42" s="125"/>
-      <c r="L42" s="125"/>
-      <c r="M42" s="125"/>
-      <c r="N42" s="126"/>
+      <c r="K42" s="135"/>
+      <c r="L42" s="135"/>
+      <c r="M42" s="135"/>
+      <c r="N42" s="136"/>
       <c r="O42" s="19"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -6292,15 +6292,15 @@
       <c r="B46" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="121" t="s">
+      <c r="C46" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="122"/>
-      <c r="E46" s="122"/>
-      <c r="F46" s="122"/>
-      <c r="G46" s="122"/>
-      <c r="H46" s="122"/>
-      <c r="I46" s="123"/>
+      <c r="D46" s="142"/>
+      <c r="E46" s="142"/>
+      <c r="F46" s="142"/>
+      <c r="G46" s="142"/>
+      <c r="H46" s="142"/>
+      <c r="I46" s="143"/>
       <c r="J46" s="11" t="s">
         <v>10</v>
       </c>
@@ -6319,25 +6319,25 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="68"/>
-      <c r="B47" s="133" t="s">
+      <c r="B47" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="134"/>
-      <c r="D47" s="134"/>
-      <c r="E47" s="134"/>
-      <c r="F47" s="135"/>
-      <c r="G47" s="124" t="s">
+      <c r="C47" s="139"/>
+      <c r="D47" s="139"/>
+      <c r="E47" s="139"/>
+      <c r="F47" s="140"/>
+      <c r="G47" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="125"/>
-      <c r="I47" s="136"/>
-      <c r="J47" s="124" t="s">
+      <c r="H47" s="135"/>
+      <c r="I47" s="137"/>
+      <c r="J47" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K47" s="125"/>
-      <c r="L47" s="125"/>
-      <c r="M47" s="125"/>
-      <c r="N47" s="126"/>
+      <c r="K47" s="135"/>
+      <c r="L47" s="135"/>
+      <c r="M47" s="135"/>
+      <c r="N47" s="136"/>
       <c r="O47" s="18"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
@@ -6406,15 +6406,15 @@
       <c r="B51" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="121" t="s">
+      <c r="C51" s="141" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="122"/>
-      <c r="G51" s="122"/>
-      <c r="H51" s="122"/>
-      <c r="I51" s="123"/>
+      <c r="D51" s="142"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="142"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="142"/>
+      <c r="I51" s="143"/>
       <c r="J51" s="11" t="s">
         <v>10</v>
       </c>
@@ -6433,25 +6433,25 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="68"/>
-      <c r="B52" s="133" t="s">
+      <c r="B52" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="134"/>
-      <c r="D52" s="134"/>
-      <c r="E52" s="134"/>
-      <c r="F52" s="135"/>
-      <c r="G52" s="124" t="s">
+      <c r="C52" s="139"/>
+      <c r="D52" s="139"/>
+      <c r="E52" s="139"/>
+      <c r="F52" s="140"/>
+      <c r="G52" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H52" s="125"/>
-      <c r="I52" s="136"/>
-      <c r="J52" s="124" t="s">
+      <c r="H52" s="135"/>
+      <c r="I52" s="137"/>
+      <c r="J52" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K52" s="125"/>
-      <c r="L52" s="125"/>
-      <c r="M52" s="125"/>
-      <c r="N52" s="126"/>
+      <c r="K52" s="135"/>
+      <c r="L52" s="135"/>
+      <c r="M52" s="135"/>
+      <c r="N52" s="136"/>
       <c r="O52" s="18"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
@@ -6535,15 +6535,15 @@
       <c r="B56" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C56" s="121" t="s">
+      <c r="C56" s="141" t="s">
         <v>212</v>
       </c>
-      <c r="D56" s="122"/>
-      <c r="E56" s="122"/>
-      <c r="F56" s="122"/>
-      <c r="G56" s="122"/>
-      <c r="H56" s="122"/>
-      <c r="I56" s="123"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="142"/>
+      <c r="F56" s="142"/>
+      <c r="G56" s="142"/>
+      <c r="H56" s="142"/>
+      <c r="I56" s="143"/>
       <c r="J56" s="11" t="s">
         <v>10</v>
       </c>
@@ -6562,25 +6562,25 @@
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="68"/>
-      <c r="B57" s="133" t="s">
+      <c r="B57" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="134"/>
-      <c r="D57" s="134"/>
-      <c r="E57" s="134"/>
-      <c r="F57" s="135"/>
-      <c r="G57" s="124" t="s">
+      <c r="C57" s="139"/>
+      <c r="D57" s="139"/>
+      <c r="E57" s="139"/>
+      <c r="F57" s="140"/>
+      <c r="G57" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="125"/>
-      <c r="I57" s="136"/>
-      <c r="J57" s="124" t="s">
+      <c r="H57" s="135"/>
+      <c r="I57" s="137"/>
+      <c r="J57" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K57" s="125"/>
-      <c r="L57" s="125"/>
-      <c r="M57" s="125"/>
-      <c r="N57" s="126"/>
+      <c r="K57" s="135"/>
+      <c r="L57" s="135"/>
+      <c r="M57" s="135"/>
+      <c r="N57" s="136"/>
       <c r="O57" s="20"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
@@ -6651,15 +6651,15 @@
       <c r="B61" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="121" t="s">
+      <c r="C61" s="141" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="122"/>
-      <c r="E61" s="122"/>
-      <c r="F61" s="122"/>
-      <c r="G61" s="122"/>
-      <c r="H61" s="122"/>
-      <c r="I61" s="123"/>
+      <c r="D61" s="142"/>
+      <c r="E61" s="142"/>
+      <c r="F61" s="142"/>
+      <c r="G61" s="142"/>
+      <c r="H61" s="142"/>
+      <c r="I61" s="143"/>
       <c r="J61" s="11" t="s">
         <v>10</v>
       </c>
@@ -6678,25 +6678,25 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="68"/>
-      <c r="B62" s="133" t="s">
+      <c r="B62" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="134"/>
-      <c r="D62" s="134"/>
-      <c r="E62" s="134"/>
-      <c r="F62" s="135"/>
-      <c r="G62" s="124" t="s">
+      <c r="C62" s="139"/>
+      <c r="D62" s="139"/>
+      <c r="E62" s="139"/>
+      <c r="F62" s="140"/>
+      <c r="G62" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="125"/>
-      <c r="I62" s="136"/>
-      <c r="J62" s="124" t="s">
+      <c r="H62" s="135"/>
+      <c r="I62" s="137"/>
+      <c r="J62" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K62" s="125"/>
-      <c r="L62" s="125"/>
-      <c r="M62" s="125"/>
-      <c r="N62" s="126"/>
+      <c r="K62" s="135"/>
+      <c r="L62" s="135"/>
+      <c r="M62" s="135"/>
+      <c r="N62" s="136"/>
       <c r="O62" s="21"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
@@ -6767,15 +6767,15 @@
       <c r="B66" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="C66" s="121" t="s">
+      <c r="C66" s="141" t="s">
         <v>225</v>
       </c>
-      <c r="D66" s="122"/>
-      <c r="E66" s="122"/>
-      <c r="F66" s="122"/>
-      <c r="G66" s="122"/>
-      <c r="H66" s="122"/>
-      <c r="I66" s="123"/>
+      <c r="D66" s="142"/>
+      <c r="E66" s="142"/>
+      <c r="F66" s="142"/>
+      <c r="G66" s="142"/>
+      <c r="H66" s="142"/>
+      <c r="I66" s="143"/>
       <c r="J66" s="11" t="s">
         <v>10</v>
       </c>
@@ -6794,25 +6794,25 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="68"/>
-      <c r="B67" s="133" t="s">
+      <c r="B67" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="134"/>
-      <c r="D67" s="134"/>
-      <c r="E67" s="134"/>
-      <c r="F67" s="135"/>
-      <c r="G67" s="124" t="s">
+      <c r="C67" s="139"/>
+      <c r="D67" s="139"/>
+      <c r="E67" s="139"/>
+      <c r="F67" s="140"/>
+      <c r="G67" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H67" s="125"/>
-      <c r="I67" s="136"/>
-      <c r="J67" s="124" t="s">
+      <c r="H67" s="135"/>
+      <c r="I67" s="137"/>
+      <c r="J67" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K67" s="125"/>
-      <c r="L67" s="125"/>
-      <c r="M67" s="125"/>
-      <c r="N67" s="126"/>
+      <c r="K67" s="135"/>
+      <c r="L67" s="135"/>
+      <c r="M67" s="135"/>
+      <c r="N67" s="136"/>
       <c r="O67" s="21"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -6898,21 +6898,21 @@
       <c r="R71" s="1"/>
     </row>
     <row r="72" spans="1:18" ht="15.75" thickBot="1">
-      <c r="B72" s="160" t="s">
+      <c r="B72" s="133" t="s">
         <v>120</v>
       </c>
-      <c r="C72" s="160"/>
-      <c r="D72" s="160"/>
-      <c r="E72" s="160"/>
-      <c r="F72" s="160"/>
-      <c r="G72" s="160"/>
-      <c r="H72" s="160"/>
-      <c r="I72" s="160"/>
-      <c r="J72" s="160"/>
-      <c r="K72" s="160"/>
-      <c r="L72" s="160"/>
-      <c r="M72" s="160"/>
-      <c r="N72" s="160"/>
+      <c r="C72" s="133"/>
+      <c r="D72" s="133"/>
+      <c r="E72" s="133"/>
+      <c r="F72" s="133"/>
+      <c r="G72" s="133"/>
+      <c r="H72" s="133"/>
+      <c r="I72" s="133"/>
+      <c r="J72" s="133"/>
+      <c r="K72" s="133"/>
+      <c r="L72" s="133"/>
+      <c r="M72" s="133"/>
+      <c r="N72" s="133"/>
       <c r="O72" s="18"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
@@ -7016,15 +7016,15 @@
       <c r="B88" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C88" s="121" t="s">
+      <c r="C88" s="141" t="s">
         <v>214</v>
       </c>
-      <c r="D88" s="122"/>
-      <c r="E88" s="122"/>
-      <c r="F88" s="122"/>
-      <c r="G88" s="122"/>
-      <c r="H88" s="122"/>
-      <c r="I88" s="123"/>
+      <c r="D88" s="142"/>
+      <c r="E88" s="142"/>
+      <c r="F88" s="142"/>
+      <c r="G88" s="142"/>
+      <c r="H88" s="142"/>
+      <c r="I88" s="143"/>
       <c r="J88" s="11" t="s">
         <v>10</v>
       </c>
@@ -7043,25 +7043,25 @@
     </row>
     <row r="89" spans="1:18">
       <c r="A89" s="67"/>
-      <c r="B89" s="133" t="s">
+      <c r="B89" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="134"/>
-      <c r="D89" s="134"/>
-      <c r="E89" s="134"/>
-      <c r="F89" s="135"/>
-      <c r="G89" s="124" t="s">
+      <c r="C89" s="139"/>
+      <c r="D89" s="139"/>
+      <c r="E89" s="139"/>
+      <c r="F89" s="140"/>
+      <c r="G89" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H89" s="125"/>
-      <c r="I89" s="136"/>
-      <c r="J89" s="124" t="s">
+      <c r="H89" s="135"/>
+      <c r="I89" s="137"/>
+      <c r="J89" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K89" s="125"/>
-      <c r="L89" s="125"/>
-      <c r="M89" s="125"/>
-      <c r="N89" s="126"/>
+      <c r="K89" s="135"/>
+      <c r="L89" s="135"/>
+      <c r="M89" s="135"/>
+      <c r="N89" s="136"/>
       <c r="O89" s="18"/>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
@@ -7132,15 +7132,15 @@
       <c r="B93" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C93" s="121" t="s">
+      <c r="C93" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="D93" s="122"/>
-      <c r="E93" s="122"/>
-      <c r="F93" s="122"/>
-      <c r="G93" s="122"/>
-      <c r="H93" s="122"/>
-      <c r="I93" s="123"/>
+      <c r="D93" s="142"/>
+      <c r="E93" s="142"/>
+      <c r="F93" s="142"/>
+      <c r="G93" s="142"/>
+      <c r="H93" s="142"/>
+      <c r="I93" s="143"/>
       <c r="J93" s="11" t="s">
         <v>10</v>
       </c>
@@ -7159,25 +7159,25 @@
     </row>
     <row r="94" spans="1:18">
       <c r="A94" s="68"/>
-      <c r="B94" s="133" t="s">
+      <c r="B94" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="134"/>
-      <c r="D94" s="134"/>
-      <c r="E94" s="134"/>
-      <c r="F94" s="135"/>
-      <c r="G94" s="124" t="s">
+      <c r="C94" s="139"/>
+      <c r="D94" s="139"/>
+      <c r="E94" s="139"/>
+      <c r="F94" s="140"/>
+      <c r="G94" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H94" s="125"/>
-      <c r="I94" s="136"/>
-      <c r="J94" s="124" t="s">
+      <c r="H94" s="135"/>
+      <c r="I94" s="137"/>
+      <c r="J94" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K94" s="125"/>
-      <c r="L94" s="125"/>
-      <c r="M94" s="125"/>
-      <c r="N94" s="126"/>
+      <c r="K94" s="135"/>
+      <c r="L94" s="135"/>
+      <c r="M94" s="135"/>
+      <c r="N94" s="136"/>
       <c r="O94" s="18"/>
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
@@ -7248,15 +7248,15 @@
       <c r="B98" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C98" s="121" t="s">
+      <c r="C98" s="141" t="s">
         <v>191</v>
       </c>
-      <c r="D98" s="122"/>
-      <c r="E98" s="122"/>
-      <c r="F98" s="122"/>
-      <c r="G98" s="122"/>
-      <c r="H98" s="122"/>
-      <c r="I98" s="123"/>
+      <c r="D98" s="142"/>
+      <c r="E98" s="142"/>
+      <c r="F98" s="142"/>
+      <c r="G98" s="142"/>
+      <c r="H98" s="142"/>
+      <c r="I98" s="143"/>
       <c r="J98" s="11" t="s">
         <v>10</v>
       </c>
@@ -7275,25 +7275,25 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99" s="68"/>
-      <c r="B99" s="133" t="s">
+      <c r="B99" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C99" s="134"/>
-      <c r="D99" s="134"/>
-      <c r="E99" s="134"/>
-      <c r="F99" s="135"/>
-      <c r="G99" s="124" t="s">
+      <c r="C99" s="139"/>
+      <c r="D99" s="139"/>
+      <c r="E99" s="139"/>
+      <c r="F99" s="140"/>
+      <c r="G99" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H99" s="125"/>
-      <c r="I99" s="136"/>
-      <c r="J99" s="124" t="s">
+      <c r="H99" s="135"/>
+      <c r="I99" s="137"/>
+      <c r="J99" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K99" s="125"/>
-      <c r="L99" s="125"/>
-      <c r="M99" s="125"/>
-      <c r="N99" s="126"/>
+      <c r="K99" s="135"/>
+      <c r="L99" s="135"/>
+      <c r="M99" s="135"/>
+      <c r="N99" s="136"/>
       <c r="O99" s="18"/>
       <c r="P99" s="1"/>
       <c r="Q99" s="1"/>
@@ -7364,15 +7364,15 @@
       <c r="B103" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C103" s="121" t="s">
+      <c r="C103" s="141" t="s">
         <v>216</v>
       </c>
-      <c r="D103" s="122"/>
-      <c r="E103" s="122"/>
-      <c r="F103" s="122"/>
-      <c r="G103" s="122"/>
-      <c r="H103" s="122"/>
-      <c r="I103" s="123"/>
+      <c r="D103" s="142"/>
+      <c r="E103" s="142"/>
+      <c r="F103" s="142"/>
+      <c r="G103" s="142"/>
+      <c r="H103" s="142"/>
+      <c r="I103" s="143"/>
       <c r="J103" s="11" t="s">
         <v>10</v>
       </c>
@@ -7391,25 +7391,25 @@
     </row>
     <row r="104" spans="1:18">
       <c r="A104" s="67"/>
-      <c r="B104" s="133" t="s">
+      <c r="B104" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C104" s="134"/>
-      <c r="D104" s="134"/>
-      <c r="E104" s="134"/>
-      <c r="F104" s="135"/>
-      <c r="G104" s="124" t="s">
+      <c r="C104" s="139"/>
+      <c r="D104" s="139"/>
+      <c r="E104" s="139"/>
+      <c r="F104" s="140"/>
+      <c r="G104" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H104" s="125"/>
-      <c r="I104" s="136"/>
-      <c r="J104" s="124" t="s">
+      <c r="H104" s="135"/>
+      <c r="I104" s="137"/>
+      <c r="J104" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K104" s="125"/>
-      <c r="L104" s="125"/>
-      <c r="M104" s="125"/>
-      <c r="N104" s="126"/>
+      <c r="K104" s="135"/>
+      <c r="L104" s="135"/>
+      <c r="M104" s="135"/>
+      <c r="N104" s="136"/>
       <c r="O104" s="18"/>
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
@@ -7513,15 +7513,15 @@
       <c r="B109" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C109" s="121" t="s">
+      <c r="C109" s="141" t="s">
         <v>217</v>
       </c>
-      <c r="D109" s="122"/>
-      <c r="E109" s="122"/>
-      <c r="F109" s="122"/>
-      <c r="G109" s="122"/>
-      <c r="H109" s="122"/>
-      <c r="I109" s="123"/>
+      <c r="D109" s="142"/>
+      <c r="E109" s="142"/>
+      <c r="F109" s="142"/>
+      <c r="G109" s="142"/>
+      <c r="H109" s="142"/>
+      <c r="I109" s="143"/>
       <c r="J109" s="11" t="s">
         <v>10</v>
       </c>
@@ -7540,25 +7540,25 @@
     </row>
     <row r="110" spans="1:18">
       <c r="A110" s="67"/>
-      <c r="B110" s="133" t="s">
+      <c r="B110" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C110" s="134"/>
-      <c r="D110" s="134"/>
-      <c r="E110" s="134"/>
-      <c r="F110" s="135"/>
-      <c r="G110" s="124" t="s">
+      <c r="C110" s="139"/>
+      <c r="D110" s="139"/>
+      <c r="E110" s="139"/>
+      <c r="F110" s="140"/>
+      <c r="G110" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H110" s="125"/>
-      <c r="I110" s="136"/>
-      <c r="J110" s="124" t="s">
+      <c r="H110" s="135"/>
+      <c r="I110" s="137"/>
+      <c r="J110" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K110" s="125"/>
-      <c r="L110" s="125"/>
-      <c r="M110" s="125"/>
-      <c r="N110" s="126"/>
+      <c r="K110" s="135"/>
+      <c r="L110" s="135"/>
+      <c r="M110" s="135"/>
+      <c r="N110" s="136"/>
       <c r="O110" s="21"/>
       <c r="P110" s="1"/>
       <c r="Q110" s="1"/>
@@ -7691,15 +7691,15 @@
       <c r="B116" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C116" s="121" t="s">
+      <c r="C116" s="141" t="s">
         <v>127</v>
       </c>
-      <c r="D116" s="122"/>
-      <c r="E116" s="122"/>
-      <c r="F116" s="122"/>
-      <c r="G116" s="122"/>
-      <c r="H116" s="122"/>
-      <c r="I116" s="123"/>
+      <c r="D116" s="142"/>
+      <c r="E116" s="142"/>
+      <c r="F116" s="142"/>
+      <c r="G116" s="142"/>
+      <c r="H116" s="142"/>
+      <c r="I116" s="143"/>
       <c r="J116" s="11" t="s">
         <v>10</v>
       </c>
@@ -7718,25 +7718,25 @@
     </row>
     <row r="117" spans="1:18">
       <c r="A117" s="18"/>
-      <c r="B117" s="133" t="s">
+      <c r="B117" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C117" s="134"/>
-      <c r="D117" s="134"/>
-      <c r="E117" s="134"/>
-      <c r="F117" s="135"/>
-      <c r="G117" s="124" t="s">
+      <c r="C117" s="139"/>
+      <c r="D117" s="139"/>
+      <c r="E117" s="139"/>
+      <c r="F117" s="140"/>
+      <c r="G117" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H117" s="125"/>
-      <c r="I117" s="136"/>
-      <c r="J117" s="124" t="s">
+      <c r="H117" s="135"/>
+      <c r="I117" s="137"/>
+      <c r="J117" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K117" s="125"/>
-      <c r="L117" s="125"/>
-      <c r="M117" s="125"/>
-      <c r="N117" s="126"/>
+      <c r="K117" s="135"/>
+      <c r="L117" s="135"/>
+      <c r="M117" s="135"/>
+      <c r="N117" s="136"/>
       <c r="O117" s="21"/>
       <c r="P117" s="23"/>
       <c r="Q117" s="23"/>
@@ -7893,15 +7893,15 @@
       <c r="B124" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C124" s="121" t="s">
+      <c r="C124" s="141" t="s">
         <v>128</v>
       </c>
-      <c r="D124" s="122"/>
-      <c r="E124" s="122"/>
-      <c r="F124" s="122"/>
-      <c r="G124" s="122"/>
-      <c r="H124" s="122"/>
-      <c r="I124" s="123"/>
+      <c r="D124" s="142"/>
+      <c r="E124" s="142"/>
+      <c r="F124" s="142"/>
+      <c r="G124" s="142"/>
+      <c r="H124" s="142"/>
+      <c r="I124" s="143"/>
       <c r="J124" s="11" t="s">
         <v>10</v>
       </c>
@@ -7920,25 +7920,25 @@
     </row>
     <row r="125" spans="1:18">
       <c r="A125" s="18"/>
-      <c r="B125" s="133" t="s">
+      <c r="B125" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C125" s="134"/>
-      <c r="D125" s="134"/>
-      <c r="E125" s="134"/>
-      <c r="F125" s="135"/>
-      <c r="G125" s="124" t="s">
+      <c r="C125" s="139"/>
+      <c r="D125" s="139"/>
+      <c r="E125" s="139"/>
+      <c r="F125" s="140"/>
+      <c r="G125" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H125" s="125"/>
-      <c r="I125" s="136"/>
-      <c r="J125" s="124" t="s">
+      <c r="H125" s="135"/>
+      <c r="I125" s="137"/>
+      <c r="J125" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K125" s="125"/>
-      <c r="L125" s="125"/>
-      <c r="M125" s="125"/>
-      <c r="N125" s="126"/>
+      <c r="K125" s="135"/>
+      <c r="L125" s="135"/>
+      <c r="M125" s="135"/>
+      <c r="N125" s="136"/>
       <c r="O125" s="21"/>
       <c r="P125" s="23"/>
       <c r="Q125" s="23"/>
@@ -8122,25 +8122,25 @@
     </row>
     <row r="133" spans="1:18">
       <c r="A133" s="18"/>
-      <c r="B133" s="133" t="s">
+      <c r="B133" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C133" s="134"/>
-      <c r="D133" s="134"/>
-      <c r="E133" s="134"/>
-      <c r="F133" s="135"/>
-      <c r="G133" s="124" t="s">
+      <c r="C133" s="139"/>
+      <c r="D133" s="139"/>
+      <c r="E133" s="139"/>
+      <c r="F133" s="140"/>
+      <c r="G133" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H133" s="125"/>
-      <c r="I133" s="136"/>
-      <c r="J133" s="124" t="s">
+      <c r="H133" s="135"/>
+      <c r="I133" s="137"/>
+      <c r="J133" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K133" s="125"/>
-      <c r="L133" s="125"/>
-      <c r="M133" s="125"/>
-      <c r="N133" s="126"/>
+      <c r="K133" s="135"/>
+      <c r="L133" s="135"/>
+      <c r="M133" s="135"/>
+      <c r="N133" s="136"/>
       <c r="O133" s="21"/>
       <c r="P133" s="23"/>
       <c r="Q133" s="23"/>
@@ -8162,13 +8162,13 @@
       </c>
       <c r="H134" s="4"/>
       <c r="I134" s="5"/>
-      <c r="J134" s="137" t="s">
+      <c r="J134" s="144" t="s">
         <v>140</v>
       </c>
-      <c r="K134" s="138"/>
-      <c r="L134" s="138"/>
-      <c r="M134" s="138"/>
-      <c r="N134" s="139"/>
+      <c r="K134" s="145"/>
+      <c r="L134" s="145"/>
+      <c r="M134" s="145"/>
+      <c r="N134" s="146"/>
       <c r="O134" s="21"/>
       <c r="P134" s="23"/>
       <c r="Q134" s="23"/>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="H135" s="1"/>
       <c r="I135" s="2"/>
-      <c r="J135" s="140"/>
+      <c r="J135" s="147"/>
       <c r="K135" s="128"/>
       <c r="L135" s="128"/>
       <c r="M135" s="128"/>
@@ -8214,7 +8214,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
       <c r="I136" s="2"/>
-      <c r="J136" s="140"/>
+      <c r="J136" s="147"/>
       <c r="K136" s="128"/>
       <c r="L136" s="128"/>
       <c r="M136" s="128"/>
@@ -8238,7 +8238,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
       <c r="I137" s="2"/>
-      <c r="J137" s="140"/>
+      <c r="J137" s="147"/>
       <c r="K137" s="128"/>
       <c r="L137" s="128"/>
       <c r="M137" s="128"/>
@@ -8262,7 +8262,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
       <c r="I138" s="2"/>
-      <c r="J138" s="140"/>
+      <c r="J138" s="147"/>
       <c r="K138" s="128"/>
       <c r="L138" s="128"/>
       <c r="M138" s="128"/>
@@ -8286,7 +8286,7 @@
       <c r="G139" s="61"/>
       <c r="H139" s="6"/>
       <c r="I139" s="14"/>
-      <c r="J139" s="141"/>
+      <c r="J139" s="148"/>
       <c r="K139" s="131"/>
       <c r="L139" s="131"/>
       <c r="M139" s="131"/>
@@ -8321,15 +8321,15 @@
       <c r="B141" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C141" s="121" t="s">
+      <c r="C141" s="141" t="s">
         <v>141</v>
       </c>
-      <c r="D141" s="122"/>
-      <c r="E141" s="122"/>
-      <c r="F141" s="122"/>
-      <c r="G141" s="122"/>
-      <c r="H141" s="122"/>
-      <c r="I141" s="123"/>
+      <c r="D141" s="142"/>
+      <c r="E141" s="142"/>
+      <c r="F141" s="142"/>
+      <c r="G141" s="142"/>
+      <c r="H141" s="142"/>
+      <c r="I141" s="143"/>
       <c r="J141" s="11" t="s">
         <v>10</v>
       </c>
@@ -8348,25 +8348,25 @@
     </row>
     <row r="142" spans="1:18">
       <c r="A142" s="18"/>
-      <c r="B142" s="133" t="s">
+      <c r="B142" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C142" s="134"/>
-      <c r="D142" s="134"/>
-      <c r="E142" s="134"/>
-      <c r="F142" s="135"/>
-      <c r="G142" s="124" t="s">
+      <c r="C142" s="139"/>
+      <c r="D142" s="139"/>
+      <c r="E142" s="139"/>
+      <c r="F142" s="140"/>
+      <c r="G142" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H142" s="125"/>
-      <c r="I142" s="136"/>
-      <c r="J142" s="124" t="s">
+      <c r="H142" s="135"/>
+      <c r="I142" s="137"/>
+      <c r="J142" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K142" s="125"/>
-      <c r="L142" s="125"/>
-      <c r="M142" s="125"/>
-      <c r="N142" s="126"/>
+      <c r="K142" s="135"/>
+      <c r="L142" s="135"/>
+      <c r="M142" s="135"/>
+      <c r="N142" s="136"/>
       <c r="O142" s="21"/>
       <c r="P142" s="23"/>
       <c r="Q142" s="23"/>
@@ -8388,13 +8388,13 @@
       </c>
       <c r="H143" s="4"/>
       <c r="I143" s="5"/>
-      <c r="J143" s="137" t="s">
+      <c r="J143" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="K143" s="138"/>
-      <c r="L143" s="138"/>
-      <c r="M143" s="138"/>
-      <c r="N143" s="139"/>
+      <c r="K143" s="145"/>
+      <c r="L143" s="145"/>
+      <c r="M143" s="145"/>
+      <c r="N143" s="146"/>
       <c r="O143" s="21"/>
       <c r="P143" s="23"/>
       <c r="Q143" s="23"/>
@@ -8416,7 +8416,7 @@
       </c>
       <c r="H144" s="1"/>
       <c r="I144" s="2"/>
-      <c r="J144" s="140"/>
+      <c r="J144" s="147"/>
       <c r="K144" s="128"/>
       <c r="L144" s="128"/>
       <c r="M144" s="128"/>
@@ -8440,7 +8440,7 @@
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
       <c r="I145" s="2"/>
-      <c r="J145" s="140"/>
+      <c r="J145" s="147"/>
       <c r="K145" s="128"/>
       <c r="L145" s="128"/>
       <c r="M145" s="128"/>
@@ -8464,7 +8464,7 @@
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
       <c r="I146" s="2"/>
-      <c r="J146" s="140"/>
+      <c r="J146" s="147"/>
       <c r="K146" s="128"/>
       <c r="L146" s="128"/>
       <c r="M146" s="128"/>
@@ -8488,7 +8488,7 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
       <c r="I147" s="2"/>
-      <c r="J147" s="140"/>
+      <c r="J147" s="147"/>
       <c r="K147" s="128"/>
       <c r="L147" s="128"/>
       <c r="M147" s="128"/>
@@ -8512,7 +8512,7 @@
       <c r="G148" s="61"/>
       <c r="H148" s="6"/>
       <c r="I148" s="14"/>
-      <c r="J148" s="141"/>
+      <c r="J148" s="148"/>
       <c r="K148" s="131"/>
       <c r="L148" s="131"/>
       <c r="M148" s="131"/>
@@ -8547,15 +8547,15 @@
       <c r="B150" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C150" s="121" t="s">
+      <c r="C150" s="141" t="s">
         <v>149</v>
       </c>
-      <c r="D150" s="122"/>
-      <c r="E150" s="122"/>
-      <c r="F150" s="122"/>
-      <c r="G150" s="122"/>
-      <c r="H150" s="122"/>
-      <c r="I150" s="123"/>
+      <c r="D150" s="142"/>
+      <c r="E150" s="142"/>
+      <c r="F150" s="142"/>
+      <c r="G150" s="142"/>
+      <c r="H150" s="142"/>
+      <c r="I150" s="143"/>
       <c r="J150" s="11" t="s">
         <v>10</v>
       </c>
@@ -8574,25 +8574,25 @@
     </row>
     <row r="151" spans="1:18">
       <c r="A151" s="18"/>
-      <c r="B151" s="133" t="s">
+      <c r="B151" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C151" s="134"/>
-      <c r="D151" s="134"/>
-      <c r="E151" s="134"/>
-      <c r="F151" s="135"/>
-      <c r="G151" s="124" t="s">
+      <c r="C151" s="139"/>
+      <c r="D151" s="139"/>
+      <c r="E151" s="139"/>
+      <c r="F151" s="140"/>
+      <c r="G151" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H151" s="125"/>
-      <c r="I151" s="136"/>
-      <c r="J151" s="124" t="s">
+      <c r="H151" s="135"/>
+      <c r="I151" s="137"/>
+      <c r="J151" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K151" s="125"/>
-      <c r="L151" s="125"/>
-      <c r="M151" s="125"/>
-      <c r="N151" s="126"/>
+      <c r="K151" s="135"/>
+      <c r="L151" s="135"/>
+      <c r="M151" s="135"/>
+      <c r="N151" s="136"/>
       <c r="O151" s="21"/>
       <c r="P151" s="23"/>
       <c r="Q151" s="23"/>
@@ -8614,13 +8614,13 @@
       </c>
       <c r="H152" s="4"/>
       <c r="I152" s="5"/>
-      <c r="J152" s="137" t="s">
+      <c r="J152" s="144" t="s">
         <v>146</v>
       </c>
-      <c r="K152" s="138"/>
-      <c r="L152" s="138"/>
-      <c r="M152" s="138"/>
-      <c r="N152" s="139"/>
+      <c r="K152" s="145"/>
+      <c r="L152" s="145"/>
+      <c r="M152" s="145"/>
+      <c r="N152" s="146"/>
       <c r="O152" s="21"/>
       <c r="P152" s="23"/>
       <c r="Q152" s="23"/>
@@ -8641,7 +8641,7 @@
       </c>
       <c r="H153" s="1"/>
       <c r="I153" s="2"/>
-      <c r="J153" s="140"/>
+      <c r="J153" s="147"/>
       <c r="K153" s="128"/>
       <c r="L153" s="128"/>
       <c r="M153" s="128"/>
@@ -8664,7 +8664,7 @@
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
       <c r="I154" s="2"/>
-      <c r="J154" s="140"/>
+      <c r="J154" s="147"/>
       <c r="K154" s="128"/>
       <c r="L154" s="128"/>
       <c r="M154" s="128"/>
@@ -8687,7 +8687,7 @@
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
       <c r="I155" s="2"/>
-      <c r="J155" s="140"/>
+      <c r="J155" s="147"/>
       <c r="K155" s="128"/>
       <c r="L155" s="128"/>
       <c r="M155" s="128"/>
@@ -8710,7 +8710,7 @@
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
       <c r="I156" s="2"/>
-      <c r="J156" s="140"/>
+      <c r="J156" s="147"/>
       <c r="K156" s="128"/>
       <c r="L156" s="128"/>
       <c r="M156" s="128"/>
@@ -8733,7 +8733,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
       <c r="I157" s="2"/>
-      <c r="J157" s="140"/>
+      <c r="J157" s="147"/>
       <c r="K157" s="128"/>
       <c r="L157" s="128"/>
       <c r="M157" s="128"/>
@@ -8756,7 +8756,7 @@
       <c r="G158" s="61"/>
       <c r="H158" s="6"/>
       <c r="I158" s="14"/>
-      <c r="J158" s="141"/>
+      <c r="J158" s="148"/>
       <c r="K158" s="131"/>
       <c r="L158" s="131"/>
       <c r="M158" s="131"/>
@@ -8790,15 +8790,15 @@
       <c r="B160" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C160" s="121" t="s">
+      <c r="C160" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="D160" s="122"/>
-      <c r="E160" s="122"/>
-      <c r="F160" s="122"/>
-      <c r="G160" s="122"/>
-      <c r="H160" s="122"/>
-      <c r="I160" s="123"/>
+      <c r="D160" s="142"/>
+      <c r="E160" s="142"/>
+      <c r="F160" s="142"/>
+      <c r="G160" s="142"/>
+      <c r="H160" s="142"/>
+      <c r="I160" s="143"/>
       <c r="J160" s="11" t="s">
         <v>10</v>
       </c>
@@ -8817,25 +8817,25 @@
     </row>
     <row r="161" spans="1:18">
       <c r="A161" s="18"/>
-      <c r="B161" s="133" t="s">
+      <c r="B161" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C161" s="134"/>
-      <c r="D161" s="134"/>
-      <c r="E161" s="134"/>
-      <c r="F161" s="135"/>
-      <c r="G161" s="124" t="s">
+      <c r="C161" s="139"/>
+      <c r="D161" s="139"/>
+      <c r="E161" s="139"/>
+      <c r="F161" s="140"/>
+      <c r="G161" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H161" s="125"/>
-      <c r="I161" s="136"/>
-      <c r="J161" s="124" t="s">
+      <c r="H161" s="135"/>
+      <c r="I161" s="137"/>
+      <c r="J161" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K161" s="125"/>
-      <c r="L161" s="125"/>
-      <c r="M161" s="125"/>
-      <c r="N161" s="126"/>
+      <c r="K161" s="135"/>
+      <c r="L161" s="135"/>
+      <c r="M161" s="135"/>
+      <c r="N161" s="136"/>
       <c r="O161" s="21"/>
       <c r="P161" s="23"/>
       <c r="Q161" s="23"/>
@@ -8857,13 +8857,13 @@
       </c>
       <c r="H162" s="4"/>
       <c r="I162" s="5"/>
-      <c r="J162" s="137" t="s">
+      <c r="J162" s="144" t="s">
         <v>151</v>
       </c>
-      <c r="K162" s="138"/>
-      <c r="L162" s="138"/>
-      <c r="M162" s="138"/>
-      <c r="N162" s="139"/>
+      <c r="K162" s="145"/>
+      <c r="L162" s="145"/>
+      <c r="M162" s="145"/>
+      <c r="N162" s="146"/>
       <c r="O162" s="21"/>
       <c r="P162" s="23"/>
       <c r="Q162" s="23"/>
@@ -8884,7 +8884,7 @@
       </c>
       <c r="H163" s="1"/>
       <c r="I163" s="2"/>
-      <c r="J163" s="140"/>
+      <c r="J163" s="147"/>
       <c r="K163" s="128"/>
       <c r="L163" s="128"/>
       <c r="M163" s="128"/>
@@ -8907,7 +8907,7 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
       <c r="I164" s="2"/>
-      <c r="J164" s="140"/>
+      <c r="J164" s="147"/>
       <c r="K164" s="128"/>
       <c r="L164" s="128"/>
       <c r="M164" s="128"/>
@@ -8930,7 +8930,7 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
       <c r="I165" s="2"/>
-      <c r="J165" s="140"/>
+      <c r="J165" s="147"/>
       <c r="K165" s="128"/>
       <c r="L165" s="128"/>
       <c r="M165" s="128"/>
@@ -8953,7 +8953,7 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
       <c r="I166" s="2"/>
-      <c r="J166" s="140"/>
+      <c r="J166" s="147"/>
       <c r="K166" s="128"/>
       <c r="L166" s="128"/>
       <c r="M166" s="128"/>
@@ -8976,7 +8976,7 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
       <c r="I167" s="2"/>
-      <c r="J167" s="140"/>
+      <c r="J167" s="147"/>
       <c r="K167" s="128"/>
       <c r="L167" s="128"/>
       <c r="M167" s="128"/>
@@ -8999,7 +8999,7 @@
       <c r="G168" s="61"/>
       <c r="H168" s="6"/>
       <c r="I168" s="14"/>
-      <c r="J168" s="141"/>
+      <c r="J168" s="148"/>
       <c r="K168" s="131"/>
       <c r="L168" s="131"/>
       <c r="M168" s="131"/>
@@ -9033,15 +9033,15 @@
       <c r="B170" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C170" s="121" t="s">
+      <c r="C170" s="141" t="s">
         <v>156</v>
       </c>
-      <c r="D170" s="122"/>
-      <c r="E170" s="122"/>
-      <c r="F170" s="122"/>
-      <c r="G170" s="122"/>
-      <c r="H170" s="122"/>
-      <c r="I170" s="123"/>
+      <c r="D170" s="142"/>
+      <c r="E170" s="142"/>
+      <c r="F170" s="142"/>
+      <c r="G170" s="142"/>
+      <c r="H170" s="142"/>
+      <c r="I170" s="143"/>
       <c r="J170" s="11" t="s">
         <v>10</v>
       </c>
@@ -9060,25 +9060,25 @@
     </row>
     <row r="171" spans="1:18">
       <c r="A171" s="18"/>
-      <c r="B171" s="133" t="s">
+      <c r="B171" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C171" s="134"/>
-      <c r="D171" s="134"/>
-      <c r="E171" s="134"/>
-      <c r="F171" s="135"/>
-      <c r="G171" s="124" t="s">
+      <c r="C171" s="139"/>
+      <c r="D171" s="139"/>
+      <c r="E171" s="139"/>
+      <c r="F171" s="140"/>
+      <c r="G171" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H171" s="125"/>
-      <c r="I171" s="136"/>
-      <c r="J171" s="124" t="s">
+      <c r="H171" s="135"/>
+      <c r="I171" s="137"/>
+      <c r="J171" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K171" s="125"/>
-      <c r="L171" s="125"/>
-      <c r="M171" s="125"/>
-      <c r="N171" s="126"/>
+      <c r="K171" s="135"/>
+      <c r="L171" s="135"/>
+      <c r="M171" s="135"/>
+      <c r="N171" s="136"/>
       <c r="O171" s="21"/>
       <c r="P171" s="23"/>
       <c r="Q171" s="23"/>
@@ -9100,13 +9100,13 @@
       </c>
       <c r="H172" s="4"/>
       <c r="I172" s="5"/>
-      <c r="J172" s="137" t="s">
+      <c r="J172" s="144" t="s">
         <v>155</v>
       </c>
-      <c r="K172" s="138"/>
-      <c r="L172" s="138"/>
-      <c r="M172" s="138"/>
-      <c r="N172" s="139"/>
+      <c r="K172" s="145"/>
+      <c r="L172" s="145"/>
+      <c r="M172" s="145"/>
+      <c r="N172" s="146"/>
       <c r="O172" s="21"/>
       <c r="P172" s="23"/>
       <c r="Q172" s="23"/>
@@ -9127,7 +9127,7 @@
       </c>
       <c r="H173" s="1"/>
       <c r="I173" s="2"/>
-      <c r="J173" s="140"/>
+      <c r="J173" s="147"/>
       <c r="K173" s="128"/>
       <c r="L173" s="128"/>
       <c r="M173" s="128"/>
@@ -9150,7 +9150,7 @@
       <c r="G174" s="6"/>
       <c r="H174" s="6"/>
       <c r="I174" s="14"/>
-      <c r="J174" s="141"/>
+      <c r="J174" s="148"/>
       <c r="K174" s="131"/>
       <c r="L174" s="131"/>
       <c r="M174" s="131"/>
@@ -9185,15 +9185,15 @@
       <c r="B176" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="C176" s="121" t="s">
+      <c r="C176" s="141" t="s">
         <v>193</v>
       </c>
-      <c r="D176" s="122"/>
-      <c r="E176" s="122"/>
-      <c r="F176" s="122"/>
-      <c r="G176" s="122"/>
-      <c r="H176" s="122"/>
-      <c r="I176" s="123"/>
+      <c r="D176" s="142"/>
+      <c r="E176" s="142"/>
+      <c r="F176" s="142"/>
+      <c r="G176" s="142"/>
+      <c r="H176" s="142"/>
+      <c r="I176" s="143"/>
       <c r="J176" s="11" t="s">
         <v>10</v>
       </c>
@@ -9212,25 +9212,25 @@
     </row>
     <row r="177" spans="1:18">
       <c r="A177" s="23"/>
-      <c r="B177" s="133" t="s">
+      <c r="B177" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C177" s="134"/>
-      <c r="D177" s="134"/>
-      <c r="E177" s="134"/>
-      <c r="F177" s="135"/>
-      <c r="G177" s="124" t="s">
+      <c r="C177" s="139"/>
+      <c r="D177" s="139"/>
+      <c r="E177" s="139"/>
+      <c r="F177" s="140"/>
+      <c r="G177" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H177" s="125"/>
-      <c r="I177" s="136"/>
-      <c r="J177" s="124" t="s">
+      <c r="H177" s="135"/>
+      <c r="I177" s="137"/>
+      <c r="J177" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K177" s="125"/>
-      <c r="L177" s="125"/>
-      <c r="M177" s="125"/>
-      <c r="N177" s="126"/>
+      <c r="K177" s="135"/>
+      <c r="L177" s="135"/>
+      <c r="M177" s="135"/>
+      <c r="N177" s="136"/>
       <c r="O177" s="20"/>
       <c r="P177" s="23"/>
       <c r="Q177" s="23"/>
@@ -9252,13 +9252,13 @@
       </c>
       <c r="H178" s="4"/>
       <c r="I178" s="5"/>
-      <c r="J178" s="137" t="s">
+      <c r="J178" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="K178" s="138"/>
-      <c r="L178" s="138"/>
-      <c r="M178" s="138"/>
-      <c r="N178" s="139"/>
+      <c r="K178" s="145"/>
+      <c r="L178" s="145"/>
+      <c r="M178" s="145"/>
+      <c r="N178" s="146"/>
       <c r="O178" s="20"/>
       <c r="P178" s="23"/>
       <c r="Q178" s="23"/>
@@ -9280,7 +9280,7 @@
       </c>
       <c r="H179" s="1"/>
       <c r="I179" s="2"/>
-      <c r="J179" s="140"/>
+      <c r="J179" s="147"/>
       <c r="K179" s="128"/>
       <c r="L179" s="128"/>
       <c r="M179" s="128"/>
@@ -9304,7 +9304,7 @@
       <c r="G180" s="6"/>
       <c r="H180" s="6"/>
       <c r="I180" s="14"/>
-      <c r="J180" s="141"/>
+      <c r="J180" s="148"/>
       <c r="K180" s="131"/>
       <c r="L180" s="131"/>
       <c r="M180" s="131"/>
@@ -9339,15 +9339,15 @@
       <c r="B182" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="C182" s="121" t="s">
+      <c r="C182" s="141" t="s">
         <v>159</v>
       </c>
-      <c r="D182" s="122"/>
-      <c r="E182" s="122"/>
-      <c r="F182" s="122"/>
-      <c r="G182" s="122"/>
-      <c r="H182" s="122"/>
-      <c r="I182" s="123"/>
+      <c r="D182" s="142"/>
+      <c r="E182" s="142"/>
+      <c r="F182" s="142"/>
+      <c r="G182" s="142"/>
+      <c r="H182" s="142"/>
+      <c r="I182" s="143"/>
       <c r="J182" s="11" t="s">
         <v>10</v>
       </c>
@@ -9366,25 +9366,25 @@
     </row>
     <row r="183" spans="1:18">
       <c r="A183" s="18"/>
-      <c r="B183" s="133" t="s">
+      <c r="B183" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C183" s="134"/>
-      <c r="D183" s="134"/>
-      <c r="E183" s="134"/>
-      <c r="F183" s="135"/>
-      <c r="G183" s="124" t="s">
+      <c r="C183" s="139"/>
+      <c r="D183" s="139"/>
+      <c r="E183" s="139"/>
+      <c r="F183" s="140"/>
+      <c r="G183" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H183" s="125"/>
-      <c r="I183" s="136"/>
-      <c r="J183" s="124" t="s">
+      <c r="H183" s="135"/>
+      <c r="I183" s="137"/>
+      <c r="J183" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K183" s="125"/>
-      <c r="L183" s="125"/>
-      <c r="M183" s="125"/>
-      <c r="N183" s="126"/>
+      <c r="K183" s="135"/>
+      <c r="L183" s="135"/>
+      <c r="M183" s="135"/>
+      <c r="N183" s="136"/>
       <c r="O183" s="21"/>
       <c r="P183" s="23"/>
       <c r="Q183" s="23"/>
@@ -9406,13 +9406,13 @@
       </c>
       <c r="H184" s="4"/>
       <c r="I184" s="5"/>
-      <c r="J184" s="137" t="s">
+      <c r="J184" s="144" t="s">
         <v>159</v>
       </c>
-      <c r="K184" s="138"/>
-      <c r="L184" s="138"/>
-      <c r="M184" s="138"/>
-      <c r="N184" s="139"/>
+      <c r="K184" s="145"/>
+      <c r="L184" s="145"/>
+      <c r="M184" s="145"/>
+      <c r="N184" s="146"/>
       <c r="O184" s="21"/>
       <c r="P184" s="23"/>
       <c r="Q184" s="23"/>
@@ -9434,7 +9434,7 @@
       </c>
       <c r="H185" s="1"/>
       <c r="I185" s="2"/>
-      <c r="J185" s="140"/>
+      <c r="J185" s="147"/>
       <c r="K185" s="128"/>
       <c r="L185" s="128"/>
       <c r="M185" s="128"/>
@@ -9458,7 +9458,7 @@
       <c r="G186" s="6"/>
       <c r="H186" s="6"/>
       <c r="I186" s="14"/>
-      <c r="J186" s="141"/>
+      <c r="J186" s="148"/>
       <c r="K186" s="131"/>
       <c r="L186" s="131"/>
       <c r="M186" s="131"/>
@@ -9493,15 +9493,15 @@
       <c r="B188" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="C188" s="121" t="s">
+      <c r="C188" s="141" t="s">
         <v>222</v>
       </c>
-      <c r="D188" s="122"/>
-      <c r="E188" s="122"/>
-      <c r="F188" s="122"/>
-      <c r="G188" s="122"/>
-      <c r="H188" s="122"/>
-      <c r="I188" s="123"/>
+      <c r="D188" s="142"/>
+      <c r="E188" s="142"/>
+      <c r="F188" s="142"/>
+      <c r="G188" s="142"/>
+      <c r="H188" s="142"/>
+      <c r="I188" s="143"/>
       <c r="J188" s="11" t="s">
         <v>10</v>
       </c>
@@ -9520,25 +9520,25 @@
     </row>
     <row r="189" spans="1:18">
       <c r="A189" s="68"/>
-      <c r="B189" s="133" t="s">
+      <c r="B189" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C189" s="134"/>
-      <c r="D189" s="134"/>
-      <c r="E189" s="134"/>
-      <c r="F189" s="135"/>
-      <c r="G189" s="124" t="s">
+      <c r="C189" s="139"/>
+      <c r="D189" s="139"/>
+      <c r="E189" s="139"/>
+      <c r="F189" s="140"/>
+      <c r="G189" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H189" s="125"/>
-      <c r="I189" s="136"/>
-      <c r="J189" s="124" t="s">
+      <c r="H189" s="135"/>
+      <c r="I189" s="137"/>
+      <c r="J189" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K189" s="125"/>
-      <c r="L189" s="125"/>
-      <c r="M189" s="125"/>
-      <c r="N189" s="126"/>
+      <c r="K189" s="135"/>
+      <c r="L189" s="135"/>
+      <c r="M189" s="135"/>
+      <c r="N189" s="136"/>
       <c r="O189" s="21"/>
       <c r="P189" s="23"/>
       <c r="Q189" s="23"/>
@@ -9560,13 +9560,13 @@
       </c>
       <c r="H190" s="4"/>
       <c r="I190" s="5"/>
-      <c r="J190" s="137" t="s">
+      <c r="J190" s="144" t="s">
         <v>222</v>
       </c>
-      <c r="K190" s="138"/>
-      <c r="L190" s="138"/>
-      <c r="M190" s="138"/>
-      <c r="N190" s="139"/>
+      <c r="K190" s="145"/>
+      <c r="L190" s="145"/>
+      <c r="M190" s="145"/>
+      <c r="N190" s="146"/>
       <c r="O190" s="21"/>
       <c r="P190" s="23"/>
       <c r="Q190" s="23"/>
@@ -9588,7 +9588,7 @@
       </c>
       <c r="H191" s="1"/>
       <c r="I191" s="2"/>
-      <c r="J191" s="140"/>
+      <c r="J191" s="147"/>
       <c r="K191" s="128"/>
       <c r="L191" s="128"/>
       <c r="M191" s="128"/>
@@ -9612,7 +9612,7 @@
       <c r="G192" s="6"/>
       <c r="H192" s="6"/>
       <c r="I192" s="14"/>
-      <c r="J192" s="141"/>
+      <c r="J192" s="148"/>
       <c r="K192" s="131"/>
       <c r="L192" s="131"/>
       <c r="M192" s="131"/>
@@ -9647,15 +9647,15 @@
       <c r="B194" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C194" s="121" t="s">
+      <c r="C194" s="141" t="s">
         <v>165</v>
       </c>
-      <c r="D194" s="122"/>
-      <c r="E194" s="122"/>
-      <c r="F194" s="122"/>
-      <c r="G194" s="122"/>
-      <c r="H194" s="122"/>
-      <c r="I194" s="123"/>
+      <c r="D194" s="142"/>
+      <c r="E194" s="142"/>
+      <c r="F194" s="142"/>
+      <c r="G194" s="142"/>
+      <c r="H194" s="142"/>
+      <c r="I194" s="143"/>
       <c r="J194" s="11" t="s">
         <v>10</v>
       </c>
@@ -9674,25 +9674,25 @@
     </row>
     <row r="195" spans="1:18">
       <c r="A195" s="18"/>
-      <c r="B195" s="133" t="s">
+      <c r="B195" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C195" s="134"/>
-      <c r="D195" s="134"/>
-      <c r="E195" s="134"/>
-      <c r="F195" s="135"/>
-      <c r="G195" s="124" t="s">
+      <c r="C195" s="139"/>
+      <c r="D195" s="139"/>
+      <c r="E195" s="139"/>
+      <c r="F195" s="140"/>
+      <c r="G195" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H195" s="125"/>
-      <c r="I195" s="136"/>
-      <c r="J195" s="124" t="s">
+      <c r="H195" s="135"/>
+      <c r="I195" s="137"/>
+      <c r="J195" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K195" s="125"/>
-      <c r="L195" s="125"/>
-      <c r="M195" s="125"/>
-      <c r="N195" s="126"/>
+      <c r="K195" s="135"/>
+      <c r="L195" s="135"/>
+      <c r="M195" s="135"/>
+      <c r="N195" s="136"/>
       <c r="O195" s="21"/>
       <c r="P195" s="23"/>
       <c r="Q195" s="23"/>
@@ -9714,13 +9714,13 @@
       </c>
       <c r="H196" s="4"/>
       <c r="I196" s="5"/>
-      <c r="J196" s="137" t="s">
+      <c r="J196" s="144" t="s">
         <v>166</v>
       </c>
-      <c r="K196" s="138"/>
-      <c r="L196" s="138"/>
-      <c r="M196" s="138"/>
-      <c r="N196" s="139"/>
+      <c r="K196" s="145"/>
+      <c r="L196" s="145"/>
+      <c r="M196" s="145"/>
+      <c r="N196" s="146"/>
       <c r="O196" s="21"/>
       <c r="P196" s="23"/>
       <c r="Q196" s="23"/>
@@ -9742,7 +9742,7 @@
       </c>
       <c r="H197" s="1"/>
       <c r="I197" s="2"/>
-      <c r="J197" s="140"/>
+      <c r="J197" s="147"/>
       <c r="K197" s="128"/>
       <c r="L197" s="128"/>
       <c r="M197" s="128"/>
@@ -9762,7 +9762,7 @@
       <c r="G198" s="6"/>
       <c r="H198" s="6"/>
       <c r="I198" s="14"/>
-      <c r="J198" s="141"/>
+      <c r="J198" s="148"/>
       <c r="K198" s="131"/>
       <c r="L198" s="131"/>
       <c r="M198" s="131"/>
@@ -9797,15 +9797,15 @@
       <c r="B200" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C200" s="121" t="s">
+      <c r="C200" s="141" t="s">
         <v>223</v>
       </c>
-      <c r="D200" s="122"/>
-      <c r="E200" s="122"/>
-      <c r="F200" s="122"/>
-      <c r="G200" s="122"/>
-      <c r="H200" s="122"/>
-      <c r="I200" s="123"/>
+      <c r="D200" s="142"/>
+      <c r="E200" s="142"/>
+      <c r="F200" s="142"/>
+      <c r="G200" s="142"/>
+      <c r="H200" s="142"/>
+      <c r="I200" s="143"/>
       <c r="J200" s="11" t="s">
         <v>10</v>
       </c>
@@ -9824,25 +9824,25 @@
     </row>
     <row r="201" spans="1:18">
       <c r="A201" s="18"/>
-      <c r="B201" s="133" t="s">
+      <c r="B201" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C201" s="134"/>
-      <c r="D201" s="134"/>
-      <c r="E201" s="134"/>
-      <c r="F201" s="135"/>
-      <c r="G201" s="124" t="s">
+      <c r="C201" s="139"/>
+      <c r="D201" s="139"/>
+      <c r="E201" s="139"/>
+      <c r="F201" s="140"/>
+      <c r="G201" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H201" s="125"/>
-      <c r="I201" s="136"/>
-      <c r="J201" s="124" t="s">
+      <c r="H201" s="135"/>
+      <c r="I201" s="137"/>
+      <c r="J201" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K201" s="125"/>
-      <c r="L201" s="125"/>
-      <c r="M201" s="125"/>
-      <c r="N201" s="126"/>
+      <c r="K201" s="135"/>
+      <c r="L201" s="135"/>
+      <c r="M201" s="135"/>
+      <c r="N201" s="136"/>
       <c r="O201" s="21"/>
       <c r="P201" s="23"/>
       <c r="Q201" s="23"/>
@@ -9864,13 +9864,13 @@
       </c>
       <c r="H202" s="4"/>
       <c r="I202" s="5"/>
-      <c r="J202" s="137" t="s">
+      <c r="J202" s="144" t="s">
         <v>167</v>
       </c>
-      <c r="K202" s="138"/>
-      <c r="L202" s="138"/>
-      <c r="M202" s="138"/>
-      <c r="N202" s="139"/>
+      <c r="K202" s="145"/>
+      <c r="L202" s="145"/>
+      <c r="M202" s="145"/>
+      <c r="N202" s="146"/>
       <c r="O202" s="21"/>
       <c r="P202" s="23"/>
       <c r="Q202" s="23"/>
@@ -9891,7 +9891,7 @@
       </c>
       <c r="H203" s="1"/>
       <c r="I203" s="2"/>
-      <c r="J203" s="140"/>
+      <c r="J203" s="147"/>
       <c r="K203" s="128"/>
       <c r="L203" s="128"/>
       <c r="M203" s="128"/>
@@ -9910,7 +9910,7 @@
       <c r="G204" s="6"/>
       <c r="H204" s="6"/>
       <c r="I204" s="14"/>
-      <c r="J204" s="141"/>
+      <c r="J204" s="148"/>
       <c r="K204" s="131"/>
       <c r="L204" s="131"/>
       <c r="M204" s="131"/>
@@ -9931,15 +9931,15 @@
       <c r="B206" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="C206" s="121" t="s">
+      <c r="C206" s="141" t="s">
         <v>168</v>
       </c>
-      <c r="D206" s="122"/>
-      <c r="E206" s="122"/>
-      <c r="F206" s="122"/>
-      <c r="G206" s="122"/>
-      <c r="H206" s="122"/>
-      <c r="I206" s="123"/>
+      <c r="D206" s="142"/>
+      <c r="E206" s="142"/>
+      <c r="F206" s="142"/>
+      <c r="G206" s="142"/>
+      <c r="H206" s="142"/>
+      <c r="I206" s="143"/>
       <c r="J206" s="11" t="s">
         <v>10</v>
       </c>
@@ -9958,25 +9958,25 @@
     </row>
     <row r="207" spans="1:18">
       <c r="A207" s="68"/>
-      <c r="B207" s="133" t="s">
+      <c r="B207" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C207" s="134"/>
-      <c r="D207" s="134"/>
-      <c r="E207" s="134"/>
-      <c r="F207" s="135"/>
-      <c r="G207" s="124" t="s">
+      <c r="C207" s="139"/>
+      <c r="D207" s="139"/>
+      <c r="E207" s="139"/>
+      <c r="F207" s="140"/>
+      <c r="G207" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H207" s="125"/>
-      <c r="I207" s="136"/>
-      <c r="J207" s="124" t="s">
+      <c r="H207" s="135"/>
+      <c r="I207" s="137"/>
+      <c r="J207" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K207" s="125"/>
-      <c r="L207" s="125"/>
-      <c r="M207" s="125"/>
-      <c r="N207" s="126"/>
+      <c r="K207" s="135"/>
+      <c r="L207" s="135"/>
+      <c r="M207" s="135"/>
+      <c r="N207" s="136"/>
       <c r="O207" s="21"/>
       <c r="P207" s="18"/>
       <c r="Q207" s="18"/>
@@ -9998,13 +9998,13 @@
       </c>
       <c r="H208" s="4"/>
       <c r="I208" s="5"/>
-      <c r="J208" s="137" t="s">
+      <c r="J208" s="144" t="s">
         <v>223</v>
       </c>
-      <c r="K208" s="138"/>
-      <c r="L208" s="138"/>
-      <c r="M208" s="138"/>
-      <c r="N208" s="139"/>
+      <c r="K208" s="145"/>
+      <c r="L208" s="145"/>
+      <c r="M208" s="145"/>
+      <c r="N208" s="146"/>
       <c r="O208" s="21"/>
       <c r="P208" s="18"/>
       <c r="Q208" s="18"/>
@@ -10026,7 +10026,7 @@
       </c>
       <c r="H209" s="1"/>
       <c r="I209" s="2"/>
-      <c r="J209" s="140"/>
+      <c r="J209" s="147"/>
       <c r="K209" s="128"/>
       <c r="L209" s="128"/>
       <c r="M209" s="128"/>
@@ -10046,7 +10046,7 @@
       <c r="G210" s="6"/>
       <c r="H210" s="6"/>
       <c r="I210" s="14"/>
-      <c r="J210" s="141"/>
+      <c r="J210" s="148"/>
       <c r="K210" s="131"/>
       <c r="L210" s="131"/>
       <c r="M210" s="131"/>
@@ -10067,15 +10067,15 @@
       <c r="B212" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="C212" s="121" t="s">
+      <c r="C212" s="141" t="s">
         <v>169</v>
       </c>
-      <c r="D212" s="122"/>
-      <c r="E212" s="122"/>
-      <c r="F212" s="122"/>
-      <c r="G212" s="122"/>
-      <c r="H212" s="122"/>
-      <c r="I212" s="123"/>
+      <c r="D212" s="142"/>
+      <c r="E212" s="142"/>
+      <c r="F212" s="142"/>
+      <c r="G212" s="142"/>
+      <c r="H212" s="142"/>
+      <c r="I212" s="143"/>
       <c r="J212" s="11" t="s">
         <v>10</v>
       </c>
@@ -10094,25 +10094,25 @@
     </row>
     <row r="213" spans="1:18">
       <c r="A213" s="68"/>
-      <c r="B213" s="133" t="s">
+      <c r="B213" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C213" s="134"/>
-      <c r="D213" s="134"/>
-      <c r="E213" s="134"/>
-      <c r="F213" s="135"/>
-      <c r="G213" s="124" t="s">
+      <c r="C213" s="139"/>
+      <c r="D213" s="139"/>
+      <c r="E213" s="139"/>
+      <c r="F213" s="140"/>
+      <c r="G213" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H213" s="125"/>
-      <c r="I213" s="136"/>
-      <c r="J213" s="124" t="s">
+      <c r="H213" s="135"/>
+      <c r="I213" s="137"/>
+      <c r="J213" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K213" s="125"/>
-      <c r="L213" s="125"/>
-      <c r="M213" s="125"/>
-      <c r="N213" s="126"/>
+      <c r="K213" s="135"/>
+      <c r="L213" s="135"/>
+      <c r="M213" s="135"/>
+      <c r="N213" s="136"/>
       <c r="O213" s="20"/>
       <c r="P213" s="1"/>
       <c r="Q213" s="1"/>
@@ -10134,13 +10134,13 @@
       </c>
       <c r="H214" s="4"/>
       <c r="I214" s="5"/>
-      <c r="J214" s="138" t="s">
+      <c r="J214" s="145" t="s">
         <v>227</v>
       </c>
-      <c r="K214" s="138"/>
-      <c r="L214" s="138"/>
-      <c r="M214" s="138"/>
-      <c r="N214" s="139"/>
+      <c r="K214" s="145"/>
+      <c r="L214" s="145"/>
+      <c r="M214" s="145"/>
+      <c r="N214" s="146"/>
       <c r="O214" s="20"/>
       <c r="P214" s="1"/>
       <c r="Q214" s="1"/>
@@ -10374,15 +10374,15 @@
       <c r="B225" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C225" s="121" t="s">
+      <c r="C225" s="141" t="s">
         <v>196</v>
       </c>
-      <c r="D225" s="122"/>
-      <c r="E225" s="122"/>
-      <c r="F225" s="122"/>
-      <c r="G225" s="122"/>
-      <c r="H225" s="122"/>
-      <c r="I225" s="123"/>
+      <c r="D225" s="142"/>
+      <c r="E225" s="142"/>
+      <c r="F225" s="142"/>
+      <c r="G225" s="142"/>
+      <c r="H225" s="142"/>
+      <c r="I225" s="143"/>
       <c r="J225" s="11" t="s">
         <v>10</v>
       </c>
@@ -10400,25 +10400,25 @@
       <c r="R225" s="17"/>
     </row>
     <row r="226" spans="1:18">
-      <c r="B226" s="133" t="s">
+      <c r="B226" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C226" s="134"/>
-      <c r="D226" s="134"/>
-      <c r="E226" s="134"/>
-      <c r="F226" s="135"/>
-      <c r="G226" s="124" t="s">
+      <c r="C226" s="139"/>
+      <c r="D226" s="139"/>
+      <c r="E226" s="139"/>
+      <c r="F226" s="140"/>
+      <c r="G226" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H226" s="125"/>
-      <c r="I226" s="136"/>
-      <c r="J226" s="124" t="s">
+      <c r="H226" s="135"/>
+      <c r="I226" s="137"/>
+      <c r="J226" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K226" s="125"/>
-      <c r="L226" s="125"/>
-      <c r="M226" s="125"/>
-      <c r="N226" s="126"/>
+      <c r="K226" s="135"/>
+      <c r="L226" s="135"/>
+      <c r="M226" s="135"/>
+      <c r="N226" s="136"/>
       <c r="O226" s="20"/>
       <c r="P226" s="1"/>
       <c r="Q226" s="1"/>
@@ -10439,13 +10439,13 @@
       </c>
       <c r="H227" s="4"/>
       <c r="I227" s="5"/>
-      <c r="J227" s="138" t="s">
+      <c r="J227" s="145" t="s">
         <v>194</v>
       </c>
-      <c r="K227" s="138"/>
-      <c r="L227" s="138"/>
-      <c r="M227" s="138"/>
-      <c r="N227" s="139"/>
+      <c r="K227" s="145"/>
+      <c r="L227" s="145"/>
+      <c r="M227" s="145"/>
+      <c r="N227" s="146"/>
       <c r="O227" s="20"/>
       <c r="P227" s="1"/>
       <c r="Q227" s="1"/>
@@ -10696,15 +10696,15 @@
       <c r="B239" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="C239" s="121" t="s">
+      <c r="C239" s="141" t="s">
         <v>182</v>
       </c>
-      <c r="D239" s="122"/>
-      <c r="E239" s="122"/>
-      <c r="F239" s="122"/>
-      <c r="G239" s="122"/>
-      <c r="H239" s="122"/>
-      <c r="I239" s="123"/>
+      <c r="D239" s="142"/>
+      <c r="E239" s="142"/>
+      <c r="F239" s="142"/>
+      <c r="G239" s="142"/>
+      <c r="H239" s="142"/>
+      <c r="I239" s="143"/>
       <c r="J239" s="11" t="s">
         <v>10</v>
       </c>
@@ -10723,25 +10723,25 @@
     </row>
     <row r="240" spans="1:18">
       <c r="A240" s="23"/>
-      <c r="B240" s="133" t="s">
+      <c r="B240" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C240" s="134"/>
-      <c r="D240" s="134"/>
-      <c r="E240" s="134"/>
-      <c r="F240" s="135"/>
-      <c r="G240" s="124" t="s">
+      <c r="C240" s="139"/>
+      <c r="D240" s="139"/>
+      <c r="E240" s="139"/>
+      <c r="F240" s="140"/>
+      <c r="G240" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H240" s="125"/>
-      <c r="I240" s="136"/>
-      <c r="J240" s="124" t="s">
+      <c r="H240" s="135"/>
+      <c r="I240" s="137"/>
+      <c r="J240" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K240" s="125"/>
-      <c r="L240" s="125"/>
-      <c r="M240" s="125"/>
-      <c r="N240" s="126"/>
+      <c r="K240" s="135"/>
+      <c r="L240" s="135"/>
+      <c r="M240" s="135"/>
+      <c r="N240" s="136"/>
       <c r="O240" s="20"/>
       <c r="P240" s="23"/>
       <c r="Q240" s="23"/>
@@ -10763,13 +10763,13 @@
       </c>
       <c r="H241" s="4"/>
       <c r="I241" s="5"/>
-      <c r="J241" s="138" t="s">
+      <c r="J241" s="145" t="s">
         <v>183</v>
       </c>
-      <c r="K241" s="138"/>
-      <c r="L241" s="138"/>
-      <c r="M241" s="138"/>
-      <c r="N241" s="139"/>
+      <c r="K241" s="145"/>
+      <c r="L241" s="145"/>
+      <c r="M241" s="145"/>
+      <c r="N241" s="146"/>
       <c r="O241" s="20"/>
       <c r="P241" s="23"/>
       <c r="Q241" s="23"/>
@@ -11200,15 +11200,15 @@
       <c r="B262" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C262" s="121" t="s">
+      <c r="C262" s="141" t="s">
         <v>115</v>
       </c>
-      <c r="D262" s="122"/>
-      <c r="E262" s="122"/>
-      <c r="F262" s="122"/>
-      <c r="G262" s="122"/>
-      <c r="H262" s="122"/>
-      <c r="I262" s="123"/>
+      <c r="D262" s="142"/>
+      <c r="E262" s="142"/>
+      <c r="F262" s="142"/>
+      <c r="G262" s="142"/>
+      <c r="H262" s="142"/>
+      <c r="I262" s="143"/>
       <c r="J262" s="11" t="s">
         <v>10</v>
       </c>
@@ -11226,25 +11226,25 @@
       <c r="R262" s="17"/>
     </row>
     <row r="263" spans="2:18">
-      <c r="B263" s="133" t="s">
+      <c r="B263" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C263" s="134"/>
-      <c r="D263" s="134"/>
-      <c r="E263" s="134"/>
-      <c r="F263" s="135"/>
-      <c r="G263" s="124" t="s">
+      <c r="C263" s="139"/>
+      <c r="D263" s="139"/>
+      <c r="E263" s="139"/>
+      <c r="F263" s="140"/>
+      <c r="G263" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H263" s="125"/>
-      <c r="I263" s="136"/>
-      <c r="J263" s="124" t="s">
+      <c r="H263" s="135"/>
+      <c r="I263" s="137"/>
+      <c r="J263" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K263" s="125"/>
-      <c r="L263" s="125"/>
-      <c r="M263" s="125"/>
-      <c r="N263" s="126"/>
+      <c r="K263" s="135"/>
+      <c r="L263" s="135"/>
+      <c r="M263" s="135"/>
+      <c r="N263" s="136"/>
       <c r="O263" s="19"/>
       <c r="P263" s="1"/>
       <c r="Q263" s="1"/>
@@ -11265,13 +11265,13 @@
       </c>
       <c r="H264" s="4"/>
       <c r="I264" s="5"/>
-      <c r="J264" s="142" t="s">
+      <c r="J264" s="149" t="s">
         <v>115</v>
       </c>
-      <c r="K264" s="143"/>
-      <c r="L264" s="143"/>
-      <c r="M264" s="143"/>
-      <c r="N264" s="144"/>
+      <c r="K264" s="150"/>
+      <c r="L264" s="150"/>
+      <c r="M264" s="150"/>
+      <c r="N264" s="151"/>
       <c r="O264" s="19"/>
       <c r="P264" s="1"/>
       <c r="Q264" s="1"/>
@@ -11290,11 +11290,11 @@
       <c r="G265" s="15"/>
       <c r="H265" s="1"/>
       <c r="I265" s="2"/>
-      <c r="J265" s="145"/>
-      <c r="K265" s="146"/>
-      <c r="L265" s="146"/>
-      <c r="M265" s="146"/>
-      <c r="N265" s="147"/>
+      <c r="J265" s="152"/>
+      <c r="K265" s="153"/>
+      <c r="L265" s="153"/>
+      <c r="M265" s="153"/>
+      <c r="N265" s="154"/>
       <c r="O265" s="19"/>
       <c r="P265" s="1"/>
       <c r="Q265" s="1"/>
@@ -11315,11 +11315,11 @@
       </c>
       <c r="H266" s="6"/>
       <c r="I266" s="14"/>
-      <c r="J266" s="148"/>
-      <c r="K266" s="149"/>
-      <c r="L266" s="149"/>
-      <c r="M266" s="149"/>
-      <c r="N266" s="150"/>
+      <c r="J266" s="155"/>
+      <c r="K266" s="156"/>
+      <c r="L266" s="156"/>
+      <c r="M266" s="156"/>
+      <c r="N266" s="157"/>
       <c r="O266" s="19"/>
       <c r="P266" s="1"/>
       <c r="Q266" s="1"/>
@@ -11348,15 +11348,15 @@
       <c r="B268" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C268" s="121" t="s">
+      <c r="C268" s="141" t="s">
         <v>117</v>
       </c>
-      <c r="D268" s="122"/>
-      <c r="E268" s="122"/>
-      <c r="F268" s="122"/>
-      <c r="G268" s="122"/>
-      <c r="H268" s="122"/>
-      <c r="I268" s="123"/>
+      <c r="D268" s="142"/>
+      <c r="E268" s="142"/>
+      <c r="F268" s="142"/>
+      <c r="G268" s="142"/>
+      <c r="H268" s="142"/>
+      <c r="I268" s="143"/>
       <c r="J268" s="11" t="s">
         <v>10</v>
       </c>
@@ -11374,25 +11374,25 @@
       <c r="R268" s="17"/>
     </row>
     <row r="269" spans="2:18">
-      <c r="B269" s="133" t="s">
+      <c r="B269" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C269" s="134"/>
-      <c r="D269" s="134"/>
-      <c r="E269" s="134"/>
-      <c r="F269" s="135"/>
-      <c r="G269" s="124" t="s">
+      <c r="C269" s="139"/>
+      <c r="D269" s="139"/>
+      <c r="E269" s="139"/>
+      <c r="F269" s="140"/>
+      <c r="G269" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="H269" s="125"/>
-      <c r="I269" s="136"/>
-      <c r="J269" s="124" t="s">
+      <c r="H269" s="135"/>
+      <c r="I269" s="137"/>
+      <c r="J269" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="K269" s="125"/>
-      <c r="L269" s="125"/>
-      <c r="M269" s="125"/>
-      <c r="N269" s="126"/>
+      <c r="K269" s="135"/>
+      <c r="L269" s="135"/>
+      <c r="M269" s="135"/>
+      <c r="N269" s="136"/>
       <c r="O269" s="19"/>
       <c r="P269" s="1"/>
       <c r="Q269" s="1"/>
@@ -11413,13 +11413,13 @@
       </c>
       <c r="H270" s="4"/>
       <c r="I270" s="5"/>
-      <c r="J270" s="151" t="s">
+      <c r="J270" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="K270" s="152"/>
-      <c r="L270" s="152"/>
-      <c r="M270" s="152"/>
-      <c r="N270" s="153"/>
+      <c r="K270" s="119"/>
+      <c r="L270" s="119"/>
+      <c r="M270" s="119"/>
+      <c r="N270" s="120"/>
       <c r="O270" s="19"/>
       <c r="P270" s="1"/>
       <c r="Q270" s="1"/>
@@ -11438,11 +11438,11 @@
       <c r="G271" s="15"/>
       <c r="H271" s="1"/>
       <c r="I271" s="2"/>
-      <c r="J271" s="154"/>
-      <c r="K271" s="155"/>
-      <c r="L271" s="155"/>
-      <c r="M271" s="155"/>
-      <c r="N271" s="156"/>
+      <c r="J271" s="121"/>
+      <c r="K271" s="122"/>
+      <c r="L271" s="122"/>
+      <c r="M271" s="122"/>
+      <c r="N271" s="123"/>
       <c r="O271" s="19"/>
       <c r="P271" s="1"/>
       <c r="Q271" s="1"/>
@@ -11461,11 +11461,11 @@
       <c r="G272" s="15"/>
       <c r="H272" s="1"/>
       <c r="I272" s="2"/>
-      <c r="J272" s="154"/>
-      <c r="K272" s="155"/>
-      <c r="L272" s="155"/>
-      <c r="M272" s="155"/>
-      <c r="N272" s="156"/>
+      <c r="J272" s="121"/>
+      <c r="K272" s="122"/>
+      <c r="L272" s="122"/>
+      <c r="M272" s="122"/>
+      <c r="N272" s="123"/>
       <c r="O272" s="19"/>
       <c r="P272" s="1"/>
       <c r="Q272" s="1"/>
@@ -11486,11 +11486,11 @@
       </c>
       <c r="H273" s="6"/>
       <c r="I273" s="14"/>
-      <c r="J273" s="157"/>
-      <c r="K273" s="158"/>
-      <c r="L273" s="158"/>
-      <c r="M273" s="158"/>
-      <c r="N273" s="159"/>
+      <c r="J273" s="124"/>
+      <c r="K273" s="125"/>
+      <c r="L273" s="125"/>
+      <c r="M273" s="125"/>
+      <c r="N273" s="126"/>
       <c r="O273" s="19"/>
       <c r="P273" s="1"/>
       <c r="Q273" s="1"/>
@@ -11553,6 +11553,159 @@
     </row>
   </sheetData>
   <mergeCells count="177">
+    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="J42:N42"/>
+    <mergeCell ref="J28:N29"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="J18:N19"/>
+    <mergeCell ref="J13:N14"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="J47:N47"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="J67:N67"/>
+    <mergeCell ref="J48:N49"/>
+    <mergeCell ref="J43:N44"/>
+    <mergeCell ref="J33:N34"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="J37:N37"/>
+    <mergeCell ref="J38:N39"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="J62:N62"/>
+    <mergeCell ref="C66:I66"/>
+    <mergeCell ref="J63:N64"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="J57:N57"/>
+    <mergeCell ref="J58:N59"/>
+    <mergeCell ref="J68:N69"/>
+    <mergeCell ref="J90:N91"/>
+    <mergeCell ref="C93:I93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="G94:I94"/>
+    <mergeCell ref="J94:N94"/>
+    <mergeCell ref="C103:I103"/>
+    <mergeCell ref="C88:I88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="G89:I89"/>
+    <mergeCell ref="J89:N89"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="G104:I104"/>
+    <mergeCell ref="J104:N104"/>
+    <mergeCell ref="J95:N96"/>
+    <mergeCell ref="C98:I98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="G99:I99"/>
+    <mergeCell ref="J99:N99"/>
+    <mergeCell ref="J100:N101"/>
+    <mergeCell ref="J105:N106"/>
+    <mergeCell ref="G142:I142"/>
+    <mergeCell ref="J177:N177"/>
+    <mergeCell ref="G177:I177"/>
+    <mergeCell ref="J142:N142"/>
+    <mergeCell ref="J134:N139"/>
+    <mergeCell ref="C109:I109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="G110:I110"/>
+    <mergeCell ref="J110:N110"/>
+    <mergeCell ref="J111:N114"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="J133:N133"/>
+    <mergeCell ref="G133:I133"/>
+    <mergeCell ref="C124:I124"/>
+    <mergeCell ref="C176:I176"/>
+    <mergeCell ref="J172:N174"/>
+    <mergeCell ref="J126:N130"/>
+    <mergeCell ref="J125:N125"/>
+    <mergeCell ref="G125:I125"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="J143:N148"/>
+    <mergeCell ref="C141:I141"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="G207:I207"/>
+    <mergeCell ref="J178:N180"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="G195:I195"/>
+    <mergeCell ref="J195:N195"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="G189:I189"/>
+    <mergeCell ref="J189:N189"/>
+    <mergeCell ref="J190:N192"/>
+    <mergeCell ref="C194:I194"/>
+    <mergeCell ref="C182:I182"/>
+    <mergeCell ref="C188:I188"/>
+    <mergeCell ref="J196:N198"/>
+    <mergeCell ref="C150:I150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="G151:I151"/>
+    <mergeCell ref="J151:N151"/>
+    <mergeCell ref="J152:N158"/>
+    <mergeCell ref="C160:I160"/>
+    <mergeCell ref="J161:N161"/>
+    <mergeCell ref="J162:N168"/>
+    <mergeCell ref="C170:I170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="G171:I171"/>
+    <mergeCell ref="J171:N171"/>
+    <mergeCell ref="G161:I161"/>
+    <mergeCell ref="G183:I183"/>
+    <mergeCell ref="J183:N183"/>
+    <mergeCell ref="J184:N186"/>
+    <mergeCell ref="C268:I268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="G269:I269"/>
+    <mergeCell ref="J269:N269"/>
+    <mergeCell ref="J264:N266"/>
+    <mergeCell ref="J213:N213"/>
+    <mergeCell ref="J214:N216"/>
+    <mergeCell ref="J227:N228"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="G263:I263"/>
+    <mergeCell ref="J263:N263"/>
+    <mergeCell ref="C262:I262"/>
+    <mergeCell ref="C225:I225"/>
+    <mergeCell ref="C239:I239"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="G240:I240"/>
+    <mergeCell ref="J240:N240"/>
+    <mergeCell ref="J241:N242"/>
     <mergeCell ref="J270:N273"/>
     <mergeCell ref="J23:N24"/>
     <mergeCell ref="J53:N54"/>
@@ -11577,159 +11730,6 @@
     <mergeCell ref="C212:I212"/>
     <mergeCell ref="B213:F213"/>
     <mergeCell ref="G213:I213"/>
-    <mergeCell ref="C268:I268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="G269:I269"/>
-    <mergeCell ref="J269:N269"/>
-    <mergeCell ref="J264:N266"/>
-    <mergeCell ref="J213:N213"/>
-    <mergeCell ref="J214:N216"/>
-    <mergeCell ref="J227:N228"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="G263:I263"/>
-    <mergeCell ref="J263:N263"/>
-    <mergeCell ref="C262:I262"/>
-    <mergeCell ref="C225:I225"/>
-    <mergeCell ref="C239:I239"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="G240:I240"/>
-    <mergeCell ref="J240:N240"/>
-    <mergeCell ref="J241:N242"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="G189:I189"/>
-    <mergeCell ref="J189:N189"/>
-    <mergeCell ref="J190:N192"/>
-    <mergeCell ref="C194:I194"/>
-    <mergeCell ref="C182:I182"/>
-    <mergeCell ref="C188:I188"/>
-    <mergeCell ref="J196:N198"/>
-    <mergeCell ref="C150:I150"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="G151:I151"/>
-    <mergeCell ref="J151:N151"/>
-    <mergeCell ref="J152:N158"/>
-    <mergeCell ref="C160:I160"/>
-    <mergeCell ref="J161:N161"/>
-    <mergeCell ref="J162:N168"/>
-    <mergeCell ref="C170:I170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="G171:I171"/>
-    <mergeCell ref="J171:N171"/>
-    <mergeCell ref="G161:I161"/>
-    <mergeCell ref="G183:I183"/>
-    <mergeCell ref="J183:N183"/>
-    <mergeCell ref="J184:N186"/>
-    <mergeCell ref="J126:N130"/>
-    <mergeCell ref="J125:N125"/>
-    <mergeCell ref="G125:I125"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="J143:N148"/>
-    <mergeCell ref="C141:I141"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="G207:I207"/>
-    <mergeCell ref="J105:N106"/>
-    <mergeCell ref="G142:I142"/>
-    <mergeCell ref="J177:N177"/>
-    <mergeCell ref="G177:I177"/>
-    <mergeCell ref="J142:N142"/>
-    <mergeCell ref="J134:N139"/>
-    <mergeCell ref="C109:I109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="G110:I110"/>
-    <mergeCell ref="J110:N110"/>
-    <mergeCell ref="J111:N114"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="J133:N133"/>
-    <mergeCell ref="G133:I133"/>
-    <mergeCell ref="C124:I124"/>
-    <mergeCell ref="J178:N180"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="G195:I195"/>
-    <mergeCell ref="J195:N195"/>
-    <mergeCell ref="C176:I176"/>
-    <mergeCell ref="J172:N174"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="G104:I104"/>
-    <mergeCell ref="J104:N104"/>
-    <mergeCell ref="J95:N96"/>
-    <mergeCell ref="C98:I98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="G99:I99"/>
-    <mergeCell ref="J99:N99"/>
-    <mergeCell ref="J100:N101"/>
-    <mergeCell ref="J57:N57"/>
-    <mergeCell ref="J58:N59"/>
-    <mergeCell ref="J68:N69"/>
-    <mergeCell ref="J90:N91"/>
-    <mergeCell ref="C93:I93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="G94:I94"/>
-    <mergeCell ref="J94:N94"/>
-    <mergeCell ref="C103:I103"/>
-    <mergeCell ref="C88:I88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="G89:I89"/>
-    <mergeCell ref="J89:N89"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="J67:N67"/>
-    <mergeCell ref="J48:N49"/>
-    <mergeCell ref="J43:N44"/>
-    <mergeCell ref="J33:N34"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="J37:N37"/>
-    <mergeCell ref="J38:N39"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="J62:N62"/>
-    <mergeCell ref="C66:I66"/>
-    <mergeCell ref="J63:N64"/>
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="J52:N52"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="J47:N47"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="J42:N42"/>
-    <mergeCell ref="J28:N29"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="J18:N19"/>
-    <mergeCell ref="J13:N14"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:N17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G34" r:id="rId1" display="Http://www.facebook.com"/>

</xml_diff>